<commit_message>
Gestion de Mensajes:100 % -------------------------------- Cambios:
Frontend
Arreglo en INDEX ya que no mostraba tildes (encode)

Backend
Gestion de Denuncias
 * Vista previa de Denuncias
  -> Publicaciones  Pronto

Gestion de Mensajes:100 %
 Derecha:
  * Vista previa de Mensajes 100%
 Izquierda:
  * Listado de Mensajes (Ver / Banear)
  * Mensaje de publicaciones (por id) (Ver)
  * Listado de Mensajes baneadas (Ver / Desbanear)

SQL:
 Se agrega Estado a la vista DATOS_CHAT, se actualiza en el diccionario de datos y el archivo CreateTables.sql
 Se agrega ID a Gestiona y se usa como primaria
</commit_message>
<xml_diff>
--- a/html/database/Diccionario de Datos.xlsx
+++ b/html/database/Diccionario de Datos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario de Datos - TABLAS" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="368">
   <si>
     <t>Nombre de la tabla</t>
   </si>
@@ -1113,6 +1113,12 @@
   </si>
   <si>
     <t>Att</t>
+  </si>
+  <si>
+    <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>Estado del mensaje</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+    <sheetView topLeftCell="A172" workbookViewId="0">
       <selection activeCell="A198" sqref="A198"/>
     </sheetView>
   </sheetViews>
@@ -6858,20 +6864,227 @@
     </row>
   </sheetData>
   <mergeCells count="252">
-    <mergeCell ref="B144:L144"/>
-    <mergeCell ref="B145:L145"/>
-    <mergeCell ref="A146:L146"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="H147:H148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="L147:L148"/>
+    <mergeCell ref="B230:L230"/>
+    <mergeCell ref="B231:L231"/>
+    <mergeCell ref="A232:L232"/>
+    <mergeCell ref="A233:A234"/>
+    <mergeCell ref="B233:B234"/>
+    <mergeCell ref="C233:C234"/>
+    <mergeCell ref="D233:D234"/>
+    <mergeCell ref="E233:E234"/>
+    <mergeCell ref="F233:F234"/>
+    <mergeCell ref="G233:G234"/>
+    <mergeCell ref="I233:I234"/>
+    <mergeCell ref="J233:K233"/>
+    <mergeCell ref="L233:L234"/>
+    <mergeCell ref="H233:H234"/>
+    <mergeCell ref="B220:L220"/>
+    <mergeCell ref="B221:L221"/>
+    <mergeCell ref="A222:L222"/>
+    <mergeCell ref="A223:A224"/>
+    <mergeCell ref="B223:B224"/>
+    <mergeCell ref="C223:C224"/>
+    <mergeCell ref="D223:D224"/>
+    <mergeCell ref="E223:E224"/>
+    <mergeCell ref="F223:F224"/>
+    <mergeCell ref="G223:G224"/>
+    <mergeCell ref="I223:I224"/>
+    <mergeCell ref="J223:K223"/>
+    <mergeCell ref="L223:L224"/>
+    <mergeCell ref="H223:H224"/>
+    <mergeCell ref="B210:L210"/>
+    <mergeCell ref="B209:L209"/>
+    <mergeCell ref="A211:L211"/>
+    <mergeCell ref="A212:A213"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:C213"/>
+    <mergeCell ref="D212:D213"/>
+    <mergeCell ref="E212:E213"/>
+    <mergeCell ref="F212:F213"/>
+    <mergeCell ref="G212:G213"/>
+    <mergeCell ref="I212:I213"/>
+    <mergeCell ref="J212:K212"/>
+    <mergeCell ref="L212:L213"/>
+    <mergeCell ref="H212:H213"/>
+    <mergeCell ref="B200:L200"/>
+    <mergeCell ref="B201:L201"/>
+    <mergeCell ref="A202:L202"/>
+    <mergeCell ref="A203:A204"/>
+    <mergeCell ref="B203:B204"/>
+    <mergeCell ref="C203:C204"/>
+    <mergeCell ref="D203:D204"/>
+    <mergeCell ref="E203:E204"/>
+    <mergeCell ref="F203:F204"/>
+    <mergeCell ref="G203:G204"/>
+    <mergeCell ref="I203:I204"/>
+    <mergeCell ref="J203:K203"/>
+    <mergeCell ref="L203:L204"/>
+    <mergeCell ref="H203:H204"/>
+    <mergeCell ref="B187:L187"/>
+    <mergeCell ref="B188:L188"/>
+    <mergeCell ref="A189:L189"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="C190:C191"/>
+    <mergeCell ref="D190:D191"/>
+    <mergeCell ref="E190:E191"/>
+    <mergeCell ref="F190:F191"/>
+    <mergeCell ref="G190:G191"/>
+    <mergeCell ref="I190:I191"/>
+    <mergeCell ref="J190:K190"/>
+    <mergeCell ref="L190:L191"/>
+    <mergeCell ref="H190:H191"/>
+    <mergeCell ref="B173:L173"/>
+    <mergeCell ref="B174:L174"/>
+    <mergeCell ref="A175:L175"/>
+    <mergeCell ref="A176:A177"/>
+    <mergeCell ref="B176:B177"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="D176:D177"/>
+    <mergeCell ref="E176:E177"/>
+    <mergeCell ref="F176:F177"/>
+    <mergeCell ref="G176:G177"/>
+    <mergeCell ref="I176:I177"/>
+    <mergeCell ref="J176:K176"/>
+    <mergeCell ref="L176:L177"/>
+    <mergeCell ref="H176:H177"/>
+    <mergeCell ref="B158:L158"/>
+    <mergeCell ref="B159:L159"/>
+    <mergeCell ref="A160:L160"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="C161:C162"/>
+    <mergeCell ref="D161:D162"/>
+    <mergeCell ref="E161:E162"/>
+    <mergeCell ref="F161:F162"/>
+    <mergeCell ref="G161:G162"/>
+    <mergeCell ref="I161:I162"/>
+    <mergeCell ref="J161:K161"/>
+    <mergeCell ref="L161:L162"/>
+    <mergeCell ref="H161:H162"/>
+    <mergeCell ref="B110:L110"/>
+    <mergeCell ref="B111:L111"/>
+    <mergeCell ref="A112:L112"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="G113:G114"/>
+    <mergeCell ref="I113:I114"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="L113:L114"/>
+    <mergeCell ref="H113:H114"/>
+    <mergeCell ref="B101:L101"/>
+    <mergeCell ref="B102:L102"/>
+    <mergeCell ref="A103:L103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="G104:G105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="L104:L105"/>
+    <mergeCell ref="H104:H105"/>
+    <mergeCell ref="B89:L89"/>
+    <mergeCell ref="B90:L90"/>
+    <mergeCell ref="A91:L91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="G92:G93"/>
+    <mergeCell ref="I92:I93"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="L92:L93"/>
+    <mergeCell ref="H92:H93"/>
+    <mergeCell ref="B128:L128"/>
+    <mergeCell ref="B129:L129"/>
+    <mergeCell ref="A130:L130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="F131:F132"/>
+    <mergeCell ref="G131:G132"/>
+    <mergeCell ref="I131:I132"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="L131:L132"/>
+    <mergeCell ref="H131:H132"/>
+    <mergeCell ref="B76:L76"/>
+    <mergeCell ref="B77:L77"/>
+    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="L79:L80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B39:L39"/>
+    <mergeCell ref="A40:L40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="B68:L68"/>
+    <mergeCell ref="B69:L69"/>
+    <mergeCell ref="A70:L70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="I71:I72"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="I51:I52"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:L52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
     <mergeCell ref="B30:L30"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="A32:L32"/>
@@ -6889,227 +7102,20 @@
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="H33:H34"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="I51:I52"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="L51:L52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="B68:L68"/>
-    <mergeCell ref="B69:L69"/>
-    <mergeCell ref="A70:L70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="I71:I72"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A40:L40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="B76:L76"/>
-    <mergeCell ref="B77:L77"/>
-    <mergeCell ref="A78:L78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="L79:L80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="B128:L128"/>
-    <mergeCell ref="B129:L129"/>
-    <mergeCell ref="A130:L130"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="F131:F132"/>
-    <mergeCell ref="G131:G132"/>
-    <mergeCell ref="I131:I132"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="L131:L132"/>
-    <mergeCell ref="H131:H132"/>
-    <mergeCell ref="B89:L89"/>
-    <mergeCell ref="B90:L90"/>
-    <mergeCell ref="A91:L91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="G92:G93"/>
-    <mergeCell ref="I92:I93"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="L92:L93"/>
-    <mergeCell ref="H92:H93"/>
-    <mergeCell ref="B101:L101"/>
-    <mergeCell ref="B102:L102"/>
-    <mergeCell ref="A103:L103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="G104:G105"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="L104:L105"/>
-    <mergeCell ref="H104:H105"/>
-    <mergeCell ref="B110:L110"/>
-    <mergeCell ref="B111:L111"/>
-    <mergeCell ref="A112:L112"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="E113:E114"/>
-    <mergeCell ref="F113:F114"/>
-    <mergeCell ref="G113:G114"/>
-    <mergeCell ref="I113:I114"/>
-    <mergeCell ref="J113:K113"/>
-    <mergeCell ref="L113:L114"/>
-    <mergeCell ref="H113:H114"/>
-    <mergeCell ref="B158:L158"/>
-    <mergeCell ref="B159:L159"/>
-    <mergeCell ref="A160:L160"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="C161:C162"/>
-    <mergeCell ref="D161:D162"/>
-    <mergeCell ref="E161:E162"/>
-    <mergeCell ref="F161:F162"/>
-    <mergeCell ref="G161:G162"/>
-    <mergeCell ref="I161:I162"/>
-    <mergeCell ref="J161:K161"/>
-    <mergeCell ref="L161:L162"/>
-    <mergeCell ref="H161:H162"/>
-    <mergeCell ref="B173:L173"/>
-    <mergeCell ref="B174:L174"/>
-    <mergeCell ref="A175:L175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="B176:B177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="D176:D177"/>
-    <mergeCell ref="E176:E177"/>
-    <mergeCell ref="F176:F177"/>
-    <mergeCell ref="G176:G177"/>
-    <mergeCell ref="I176:I177"/>
-    <mergeCell ref="J176:K176"/>
-    <mergeCell ref="L176:L177"/>
-    <mergeCell ref="H176:H177"/>
-    <mergeCell ref="B187:L187"/>
-    <mergeCell ref="B188:L188"/>
-    <mergeCell ref="A189:L189"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="C190:C191"/>
-    <mergeCell ref="D190:D191"/>
-    <mergeCell ref="E190:E191"/>
-    <mergeCell ref="F190:F191"/>
-    <mergeCell ref="G190:G191"/>
-    <mergeCell ref="I190:I191"/>
-    <mergeCell ref="J190:K190"/>
-    <mergeCell ref="L190:L191"/>
-    <mergeCell ref="H190:H191"/>
-    <mergeCell ref="B200:L200"/>
-    <mergeCell ref="B201:L201"/>
-    <mergeCell ref="A202:L202"/>
-    <mergeCell ref="A203:A204"/>
-    <mergeCell ref="B203:B204"/>
-    <mergeCell ref="C203:C204"/>
-    <mergeCell ref="D203:D204"/>
-    <mergeCell ref="E203:E204"/>
-    <mergeCell ref="F203:F204"/>
-    <mergeCell ref="G203:G204"/>
-    <mergeCell ref="I203:I204"/>
-    <mergeCell ref="J203:K203"/>
-    <mergeCell ref="L203:L204"/>
-    <mergeCell ref="H203:H204"/>
-    <mergeCell ref="B210:L210"/>
-    <mergeCell ref="B209:L209"/>
-    <mergeCell ref="A211:L211"/>
-    <mergeCell ref="A212:A213"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:C213"/>
-    <mergeCell ref="D212:D213"/>
-    <mergeCell ref="E212:E213"/>
-    <mergeCell ref="F212:F213"/>
-    <mergeCell ref="G212:G213"/>
-    <mergeCell ref="I212:I213"/>
-    <mergeCell ref="J212:K212"/>
-    <mergeCell ref="L212:L213"/>
-    <mergeCell ref="H212:H213"/>
-    <mergeCell ref="B220:L220"/>
-    <mergeCell ref="B221:L221"/>
-    <mergeCell ref="A222:L222"/>
-    <mergeCell ref="A223:A224"/>
-    <mergeCell ref="B223:B224"/>
-    <mergeCell ref="C223:C224"/>
-    <mergeCell ref="D223:D224"/>
-    <mergeCell ref="E223:E224"/>
-    <mergeCell ref="F223:F224"/>
-    <mergeCell ref="G223:G224"/>
-    <mergeCell ref="I223:I224"/>
-    <mergeCell ref="J223:K223"/>
-    <mergeCell ref="L223:L224"/>
-    <mergeCell ref="H223:H224"/>
-    <mergeCell ref="B230:L230"/>
-    <mergeCell ref="B231:L231"/>
-    <mergeCell ref="A232:L232"/>
-    <mergeCell ref="A233:A234"/>
-    <mergeCell ref="B233:B234"/>
-    <mergeCell ref="C233:C234"/>
-    <mergeCell ref="D233:D234"/>
-    <mergeCell ref="E233:E234"/>
-    <mergeCell ref="F233:F234"/>
-    <mergeCell ref="G233:G234"/>
-    <mergeCell ref="I233:I234"/>
-    <mergeCell ref="J233:K233"/>
-    <mergeCell ref="L233:L234"/>
-    <mergeCell ref="H233:H234"/>
+    <mergeCell ref="B144:L144"/>
+    <mergeCell ref="B145:L145"/>
+    <mergeCell ref="A146:L146"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="H147:H148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="J147:K147"/>
+    <mergeCell ref="L147:L148"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -7118,10 +7124,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I354"/>
+  <dimension ref="A1:I355"/>
   <sheetViews>
-    <sheetView topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149:G149"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="F286" sqref="F286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11735,26 +11741,36 @@
         <v>297</v>
       </c>
     </row>
-    <row r="285" spans="1:7" ht="15.75" thickBot="1"/>
+    <row r="285" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A285" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C285" s="3">
+        <v>15</v>
+      </c>
+      <c r="D285" s="3"/>
+      <c r="E285" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F285" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="G285" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
     <row r="286" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A286" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B286" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C286" s="20"/>
-      <c r="D286" s="20"/>
-      <c r="E286" s="20"/>
-      <c r="F286" s="20"/>
-      <c r="G286" s="21"/>
+      <c r="F286" s="7"/>
     </row>
     <row r="287" spans="1:7" ht="15.75" thickBot="1">
       <c r="A287" s="1" t="s">
-        <v>2</v>
+        <v>154</v>
       </c>
       <c r="B287" s="19" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C287" s="20"/>
       <c r="D287" s="20"/>
@@ -11763,72 +11779,64 @@
       <c r="G287" s="21"/>
     </row>
     <row r="288" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A288" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B288" s="20"/>
+      <c r="A288" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B288" s="19" t="s">
+        <v>298</v>
+      </c>
       <c r="C288" s="20"/>
       <c r="D288" s="20"/>
       <c r="E288" s="20"/>
       <c r="F288" s="20"/>
       <c r="G288" s="21"/>
     </row>
-    <row r="289" spans="1:7">
-      <c r="A289" s="22" t="s">
+    <row r="289" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A289" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B289" s="20"/>
+      <c r="C289" s="20"/>
+      <c r="D289" s="20"/>
+      <c r="E289" s="20"/>
+      <c r="F289" s="20"/>
+      <c r="G289" s="21"/>
+    </row>
+    <row r="290" spans="1:7">
+      <c r="A290" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B289" s="22" t="s">
+      <c r="B290" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C289" s="22" t="s">
+      <c r="C290" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D289" s="22" t="s">
+      <c r="D290" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="E289" s="22" t="s">
+      <c r="E290" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F289" s="22" t="s">
+      <c r="F290" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G289" s="22" t="s">
+      <c r="G290" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="290" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A290" s="23"/>
-      <c r="B290" s="23"/>
-      <c r="C290" s="23"/>
-      <c r="D290" s="23"/>
-      <c r="E290" s="23"/>
-      <c r="F290" s="23"/>
-      <c r="G290" s="23"/>
-    </row>
     <row r="291" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A291" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C291" s="3">
-        <v>20</v>
-      </c>
-      <c r="D291" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E291" s="3"/>
-      <c r="F291" s="3">
-        <v>0</v>
-      </c>
-      <c r="G291" s="3" t="s">
-        <v>287</v>
-      </c>
+      <c r="A291" s="23"/>
+      <c r="B291" s="23"/>
+      <c r="C291" s="23"/>
+      <c r="D291" s="23"/>
+      <c r="E291" s="23"/>
+      <c r="F291" s="23"/>
+      <c r="G291" s="23"/>
     </row>
     <row r="292" spans="1:7" ht="15.75" thickBot="1">
       <c r="A292" s="3" t="s">
-        <v>60</v>
+        <v>282</v>
       </c>
       <c r="B292" s="3" t="s">
         <v>102</v>
@@ -11840,211 +11848,219 @@
         <v>159</v>
       </c>
       <c r="E292" s="3"/>
-      <c r="F292" s="3"/>
+      <c r="F292" s="3">
+        <v>0</v>
+      </c>
       <c r="G292" s="3" t="s">
-        <v>181</v>
+        <v>287</v>
       </c>
     </row>
     <row r="293" spans="1:7" ht="15.75" thickBot="1">
       <c r="A293" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C293" s="3">
-        <v>150</v>
-      </c>
-      <c r="D293" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D293" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E293" s="3"/>
-      <c r="F293" s="4"/>
+      <c r="F293" s="3"/>
       <c r="G293" s="3" t="s">
-        <v>289</v>
+        <v>181</v>
       </c>
     </row>
     <row r="294" spans="1:7" ht="15.75" thickBot="1">
       <c r="A294" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C294" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="C294" s="3">
+        <v>150</v>
+      </c>
       <c r="D294" s="3"/>
       <c r="E294" s="3"/>
-      <c r="F294" s="3" t="s">
-        <v>204</v>
-      </c>
+      <c r="F294" s="4"/>
       <c r="G294" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="295" spans="1:7" ht="15.75" thickBot="1">
       <c r="A295" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C295" s="3">
-        <v>150</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C295" s="3"/>
       <c r="D295" s="3"/>
-      <c r="E295" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F295" s="3"/>
+      <c r="E295" s="3"/>
+      <c r="F295" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="G295" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="296" spans="1:7" ht="15.75" thickBot="1">
       <c r="A296" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C296" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="C296" s="3">
+        <v>150</v>
+      </c>
       <c r="D296" s="3"/>
-      <c r="E296" s="3"/>
-      <c r="F296" s="3" t="s">
-        <v>204</v>
-      </c>
+      <c r="E296" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F296" s="3"/>
       <c r="G296" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="297" spans="1:7" ht="15.75" thickBot="1">
       <c r="A297" s="3" t="s">
-        <v>222</v>
+        <v>68</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C297" s="3">
-        <v>20</v>
-      </c>
-      <c r="D297" s="3" t="s">
-        <v>159</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C297" s="3"/>
+      <c r="D297" s="3"/>
       <c r="E297" s="3"/>
-      <c r="F297" s="3">
-        <v>0</v>
+      <c r="F297" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="G297" s="3" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
     </row>
     <row r="298" spans="1:7" ht="15.75" thickBot="1">
       <c r="A298" s="3" t="s">
-        <v>283</v>
+        <v>222</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C298" s="3">
-        <v>10</v>
-      </c>
-      <c r="D298" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D298" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E298" s="3"/>
-      <c r="F298" s="3"/>
+      <c r="F298" s="3">
+        <v>0</v>
+      </c>
       <c r="G298" s="3" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="299" spans="1:7" ht="15.75" thickBot="1">
       <c r="A299" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B299" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C299" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D299" s="3"/>
       <c r="E299" s="3"/>
       <c r="F299" s="3"/>
       <c r="G299" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="300" spans="1:7" ht="15.75" thickBot="1">
       <c r="A300" s="3" t="s">
-        <v>221</v>
+        <v>284</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="C300" s="3">
         <v>20</v>
       </c>
-      <c r="D300" s="3" t="s">
-        <v>159</v>
-      </c>
+      <c r="D300" s="3"/>
       <c r="E300" s="3"/>
-      <c r="F300" s="3">
-        <v>0</v>
-      </c>
+      <c r="F300" s="3"/>
       <c r="G300" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="301" spans="1:7" ht="15.75" thickBot="1">
       <c r="A301" s="3" t="s">
-        <v>285</v>
+        <v>221</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C301" s="3">
-        <v>10</v>
-      </c>
-      <c r="D301" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D301" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E301" s="3"/>
-      <c r="F301" s="3"/>
+      <c r="F301" s="3">
+        <v>0</v>
+      </c>
       <c r="G301" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="302" spans="1:7" ht="15.75" thickBot="1">
       <c r="A302" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B302" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C302" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D302" s="3"/>
       <c r="E302" s="3"/>
       <c r="F302" s="3"/>
       <c r="G302" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A303" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B303" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C303" s="3">
+        <v>20</v>
+      </c>
+      <c r="D303" s="3"/>
+      <c r="E303" s="3"/>
+      <c r="F303" s="3"/>
+      <c r="G303" s="3" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="303" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="304" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A304" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B304" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="C304" s="20"/>
-      <c r="D304" s="20"/>
-      <c r="E304" s="20"/>
-      <c r="F304" s="20"/>
-      <c r="G304" s="21"/>
-    </row>
+    <row r="304" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="305" spans="1:7" ht="15.75" thickBot="1">
       <c r="A305" s="1" t="s">
-        <v>2</v>
+        <v>154</v>
       </c>
       <c r="B305" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C305" s="20"/>
       <c r="D305" s="20"/>
@@ -12053,72 +12069,64 @@
       <c r="G305" s="21"/>
     </row>
     <row r="306" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A306" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B306" s="20"/>
+      <c r="A306" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B306" s="19" t="s">
+        <v>300</v>
+      </c>
       <c r="C306" s="20"/>
       <c r="D306" s="20"/>
       <c r="E306" s="20"/>
       <c r="F306" s="20"/>
       <c r="G306" s="21"/>
     </row>
-    <row r="307" spans="1:7">
-      <c r="A307" s="22" t="s">
+    <row r="307" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A307" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B307" s="20"/>
+      <c r="C307" s="20"/>
+      <c r="D307" s="20"/>
+      <c r="E307" s="20"/>
+      <c r="F307" s="20"/>
+      <c r="G307" s="21"/>
+    </row>
+    <row r="308" spans="1:7">
+      <c r="A308" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B307" s="22" t="s">
+      <c r="B308" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C307" s="22" t="s">
+      <c r="C308" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D307" s="22" t="s">
+      <c r="D308" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="E307" s="22" t="s">
+      <c r="E308" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F307" s="22" t="s">
+      <c r="F308" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G307" s="22" t="s">
+      <c r="G308" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="308" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A308" s="23"/>
-      <c r="B308" s="23"/>
-      <c r="C308" s="23"/>
-      <c r="D308" s="23"/>
-      <c r="E308" s="23"/>
-      <c r="F308" s="23"/>
-      <c r="G308" s="23"/>
-    </row>
     <row r="309" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A309" s="3" t="s">
+      <c r="A309" s="23"/>
+      <c r="B309" s="23"/>
+      <c r="C309" s="23"/>
+      <c r="D309" s="23"/>
+      <c r="E309" s="23"/>
+      <c r="F309" s="23"/>
+      <c r="G309" s="23"/>
+    </row>
+    <row r="310" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A310" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B309" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C309" s="1">
-        <v>20</v>
-      </c>
-      <c r="D309" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E309" s="3"/>
-      <c r="F309" s="3">
-        <v>0</v>
-      </c>
-      <c r="G309" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="310" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A310" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>102</v>
@@ -12130,14 +12138,16 @@
         <v>159</v>
       </c>
       <c r="E310" s="3"/>
-      <c r="F310" s="3"/>
+      <c r="F310" s="3">
+        <v>0</v>
+      </c>
       <c r="G310" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="311" spans="1:7" ht="15.75" thickBot="1">
       <c r="A311" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>102</v>
@@ -12151,376 +12161,382 @@
       <c r="E311" s="3"/>
       <c r="F311" s="3"/>
       <c r="G311" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="312" spans="1:7" ht="15.75" thickBot="1">
       <c r="A312" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B312" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C312" s="3">
-        <v>15</v>
-      </c>
-      <c r="D312" s="3"/>
-      <c r="E312" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F312" s="3" t="s">
-        <v>321</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C312" s="1">
+        <v>20</v>
+      </c>
+      <c r="D312" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E312" s="3"/>
+      <c r="F312" s="3"/>
       <c r="G312" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="313" spans="1:7" ht="15.75" thickBot="1">
       <c r="A313" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B313" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C313" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C313" s="3">
+        <v>15</v>
+      </c>
       <c r="D313" s="3"/>
-      <c r="E313" s="3"/>
+      <c r="E313" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="F313" s="3" t="s">
-        <v>204</v>
+        <v>321</v>
       </c>
       <c r="G313" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="314" spans="1:7" ht="15.75" thickBot="1">
       <c r="A314" s="1" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C314" s="1">
-        <v>1</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C314" s="1"/>
       <c r="D314" s="3"/>
-      <c r="E314" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F314" s="3">
-        <v>0</v>
+      <c r="E314" s="3"/>
+      <c r="F314" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="G314" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="315" spans="1:7" ht="15.75" thickBot="1">
       <c r="A315" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C315" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="C315" s="1">
+        <v>1</v>
+      </c>
       <c r="D315" s="3"/>
       <c r="E315" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F315" s="3"/>
+      <c r="F315" s="3">
+        <v>0</v>
+      </c>
       <c r="G315" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="316" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A316" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B316" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C316" s="3">
-        <v>1</v>
-      </c>
+      <c r="A316" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C316" s="1"/>
       <c r="D316" s="3"/>
       <c r="E316" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F316" s="3">
-        <v>0</v>
-      </c>
+      <c r="F316" s="3"/>
       <c r="G316" s="3" t="s">
-        <v>202</v>
+        <v>307</v>
       </c>
     </row>
     <row r="317" spans="1:7" ht="15.75" thickBot="1">
       <c r="A317" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="B317" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C317" s="1">
-        <v>20</v>
-      </c>
-      <c r="D317" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E317" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="B317" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C317" s="3">
+        <v>1</v>
+      </c>
+      <c r="D317" s="3"/>
+      <c r="E317" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="F317" s="3">
         <v>0</v>
       </c>
       <c r="G317" s="3" t="s">
-        <v>323</v>
+        <v>202</v>
       </c>
     </row>
     <row r="318" spans="1:7" ht="15.75" thickBot="1">
       <c r="A318" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B318" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C318" s="3">
+        <v>308</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C318" s="1">
         <v>20</v>
       </c>
-      <c r="D318" s="3"/>
+      <c r="D318" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E318" s="3"/>
-      <c r="F318" s="3"/>
+      <c r="F318" s="3">
+        <v>0</v>
+      </c>
       <c r="G318" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="319" spans="1:7" ht="15.75" thickBot="1">
       <c r="A319" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B319" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C319" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D319" s="3"/>
       <c r="E319" s="3"/>
       <c r="F319" s="3"/>
       <c r="G319" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="320" spans="1:7" ht="15.75" thickBot="1">
       <c r="A320" s="3" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C320" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="C320" s="3">
+        <v>50</v>
+      </c>
       <c r="D320" s="3"/>
       <c r="E320" s="3"/>
       <c r="F320" s="3"/>
       <c r="G320" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="321" spans="1:7" ht="15.75" thickBot="1">
       <c r="A321" s="3" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
-      <c r="E321" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F321" s="3">
-        <v>1</v>
-      </c>
+      <c r="E321" s="3"/>
+      <c r="F321" s="3"/>
       <c r="G321" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="322" spans="1:7" ht="15.75" thickBot="1">
       <c r="A322" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C322" s="3">
-        <v>50</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C322" s="3"/>
       <c r="D322" s="3"/>
       <c r="E322" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F322" s="3" t="s">
-        <v>186</v>
+      <c r="F322" s="3">
+        <v>1</v>
       </c>
       <c r="G322" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="323" spans="1:7" ht="15.75" thickBot="1">
       <c r="A323" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C323" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C323" s="3">
+        <v>50</v>
+      </c>
       <c r="D323" s="3"/>
-      <c r="E323" s="3"/>
-      <c r="F323" s="3"/>
+      <c r="E323" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F323" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="G323" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="324" spans="1:7" ht="15.75" thickBot="1">
       <c r="A324" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="B324" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C324" s="1">
-        <v>20</v>
-      </c>
-      <c r="D324" s="3" t="s">
-        <v>159</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="B324" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C324" s="1"/>
+      <c r="D324" s="3"/>
       <c r="E324" s="3"/>
-      <c r="F324" s="3">
-        <v>0</v>
-      </c>
+      <c r="F324" s="3"/>
       <c r="G324" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="325" spans="1:7" ht="15.75" thickBot="1">
       <c r="A325" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="B325" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C325" s="3">
+        <v>314</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C325" s="1">
         <v>20</v>
       </c>
-      <c r="D325" s="3"/>
+      <c r="D325" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E325" s="3"/>
-      <c r="F325" s="3"/>
+      <c r="F325" s="3">
+        <v>0</v>
+      </c>
       <c r="G325" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="326" spans="1:7" ht="15.75" thickBot="1">
       <c r="A326" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B326" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C326" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D326" s="3"/>
       <c r="E326" s="3"/>
       <c r="F326" s="3"/>
       <c r="G326" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="327" spans="1:7" ht="15.75" thickBot="1">
       <c r="A327" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C327" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="C327" s="3">
+        <v>50</v>
+      </c>
       <c r="D327" s="3"/>
       <c r="E327" s="3"/>
       <c r="F327" s="3"/>
       <c r="G327" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="328" spans="1:7" ht="15.75" thickBot="1">
       <c r="A328" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
-      <c r="E328" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F328" s="3">
-        <v>1</v>
-      </c>
+      <c r="E328" s="3"/>
+      <c r="F328" s="3"/>
       <c r="G328" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="329" spans="1:7" ht="15.75" thickBot="1">
       <c r="A329" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C329" s="3">
-        <v>50</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C329" s="3"/>
       <c r="D329" s="3"/>
       <c r="E329" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F329" s="3" t="s">
-        <v>186</v>
+      <c r="F329" s="3">
+        <v>1</v>
       </c>
       <c r="G329" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="330" spans="1:7" ht="15.75" thickBot="1">
       <c r="A330" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B330" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C330" s="3">
+        <v>50</v>
+      </c>
+      <c r="D330" s="3"/>
+      <c r="E330" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F330" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G330" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A331" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B330" s="3" t="s">
+      <c r="B331" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C330" s="1"/>
-      <c r="D330" s="3"/>
-      <c r="E330" s="3"/>
-      <c r="F330" s="3"/>
-      <c r="G330" s="3" t="s">
+      <c r="C331" s="1"/>
+      <c r="D331" s="3"/>
+      <c r="E331" s="3"/>
+      <c r="F331" s="3"/>
+      <c r="G331" s="3" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="331" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="332" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A332" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B332" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="C332" s="20"/>
-      <c r="D332" s="20"/>
-      <c r="E332" s="20"/>
-      <c r="F332" s="20"/>
-      <c r="G332" s="21"/>
-    </row>
+    <row r="332" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="333" spans="1:7" ht="15.75" thickBot="1">
       <c r="A333" s="1" t="s">
-        <v>2</v>
+        <v>154</v>
       </c>
       <c r="B333" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C333" s="20"/>
       <c r="D333" s="20"/>
@@ -12529,144 +12545,144 @@
       <c r="G333" s="21"/>
     </row>
     <row r="334" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A334" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B334" s="20"/>
+      <c r="A334" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B334" s="19" t="s">
+        <v>338</v>
+      </c>
       <c r="C334" s="20"/>
       <c r="D334" s="20"/>
       <c r="E334" s="20"/>
       <c r="F334" s="20"/>
       <c r="G334" s="21"/>
     </row>
-    <row r="335" spans="1:7">
-      <c r="A335" s="22" t="s">
+    <row r="335" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A335" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B335" s="20"/>
+      <c r="C335" s="20"/>
+      <c r="D335" s="20"/>
+      <c r="E335" s="20"/>
+      <c r="F335" s="20"/>
+      <c r="G335" s="21"/>
+    </row>
+    <row r="336" spans="1:7">
+      <c r="A336" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B335" s="22" t="s">
+      <c r="B336" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C335" s="22" t="s">
+      <c r="C336" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D335" s="22" t="s">
+      <c r="D336" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="E335" s="22" t="s">
+      <c r="E336" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F335" s="22" t="s">
+      <c r="F336" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G335" s="22" t="s">
+      <c r="G336" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="336" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A336" s="23"/>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
-      <c r="D336" s="23"/>
-      <c r="E336" s="23"/>
-      <c r="F336" s="23"/>
-      <c r="G336" s="23"/>
-    </row>
     <row r="337" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A337" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B337" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C337" s="1">
-        <v>20</v>
-      </c>
-      <c r="D337" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E337" s="3"/>
-      <c r="F337" s="3"/>
-      <c r="G337" s="3" t="s">
-        <v>190</v>
-      </c>
+      <c r="A337" s="23"/>
+      <c r="B337" s="23"/>
+      <c r="C337" s="23"/>
+      <c r="D337" s="23"/>
+      <c r="E337" s="23"/>
+      <c r="F337" s="23"/>
+      <c r="G337" s="23"/>
     </row>
     <row r="338" spans="1:7" ht="15.75" thickBot="1">
       <c r="A338" s="3" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C338" s="1">
-        <v>50</v>
-      </c>
-      <c r="D338" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D338" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E338" s="3"/>
       <c r="F338" s="3"/>
       <c r="G338" s="3" t="s">
-        <v>272</v>
+        <v>190</v>
       </c>
     </row>
     <row r="339" spans="1:7" ht="15.75" thickBot="1">
       <c r="A339" s="3" t="s">
-        <v>339</v>
+        <v>34</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="C339" s="1">
-        <v>20</v>
-      </c>
-      <c r="D339" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E339" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D339" s="3"/>
+      <c r="E339" s="3"/>
       <c r="F339" s="3"/>
       <c r="G339" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="340" spans="1:7" ht="15.75" thickBot="1">
       <c r="A340" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C340" s="1">
-        <v>50</v>
-      </c>
-      <c r="D340" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D340" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E340" s="3" t="s">
         <v>82</v>
       </c>
       <c r="F340" s="3"/>
       <c r="G340" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A341" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C341" s="1">
+        <v>50</v>
+      </c>
+      <c r="D341" s="3"/>
+      <c r="E341" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F341" s="3"/>
+      <c r="G341" s="3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="341" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="342" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A342" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B342" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="C342" s="20"/>
-      <c r="D342" s="20"/>
-      <c r="E342" s="20"/>
-      <c r="F342" s="20"/>
-      <c r="G342" s="21"/>
-    </row>
+    <row r="342" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="343" spans="1:7" ht="15.75" thickBot="1">
       <c r="A343" s="1" t="s">
-        <v>2</v>
+        <v>154</v>
       </c>
       <c r="B343" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C343" s="20"/>
       <c r="D343" s="20"/>
@@ -12675,70 +12691,64 @@
       <c r="G343" s="21"/>
     </row>
     <row r="344" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A344" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B344" s="20"/>
+      <c r="A344" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B344" s="19" t="s">
+        <v>343</v>
+      </c>
       <c r="C344" s="20"/>
       <c r="D344" s="20"/>
       <c r="E344" s="20"/>
       <c r="F344" s="20"/>
       <c r="G344" s="21"/>
     </row>
-    <row r="345" spans="1:7">
-      <c r="A345" s="22" t="s">
+    <row r="345" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A345" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B345" s="20"/>
+      <c r="C345" s="20"/>
+      <c r="D345" s="20"/>
+      <c r="E345" s="20"/>
+      <c r="F345" s="20"/>
+      <c r="G345" s="21"/>
+    </row>
+    <row r="346" spans="1:7">
+      <c r="A346" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B345" s="22" t="s">
+      <c r="B346" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C345" s="22" t="s">
+      <c r="C346" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D345" s="22" t="s">
+      <c r="D346" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="E345" s="22" t="s">
+      <c r="E346" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F345" s="22" t="s">
+      <c r="F346" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G345" s="22" t="s">
+      <c r="G346" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="346" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A346" s="23"/>
-      <c r="B346" s="23"/>
-      <c r="C346" s="23"/>
-      <c r="D346" s="23"/>
-      <c r="E346" s="23"/>
-      <c r="F346" s="23"/>
-      <c r="G346" s="23"/>
-    </row>
     <row r="347" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A347" s="3" t="s">
+      <c r="A347" s="23"/>
+      <c r="B347" s="23"/>
+      <c r="C347" s="23"/>
+      <c r="D347" s="23"/>
+      <c r="E347" s="23"/>
+      <c r="F347" s="23"/>
+      <c r="G347" s="23"/>
+    </row>
+    <row r="348" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A348" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B347" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C347" s="1">
-        <v>20</v>
-      </c>
-      <c r="D347" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E347" s="3"/>
-      <c r="F347" s="3"/>
-      <c r="G347" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="348" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A348" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>102</v>
@@ -12752,109 +12762,338 @@
       <c r="E348" s="3"/>
       <c r="F348" s="3"/>
       <c r="G348" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="349" spans="1:7" ht="15.75" thickBot="1">
       <c r="A349" s="1" t="s">
-        <v>344</v>
+        <v>59</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C349" s="1"/>
-      <c r="D349" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="C349" s="1">
+        <v>20</v>
+      </c>
+      <c r="D349" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="E349" s="3"/>
-      <c r="F349" s="3" t="s">
-        <v>204</v>
-      </c>
+      <c r="F349" s="3"/>
       <c r="G349" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="350" spans="1:7" ht="15.75" thickBot="1">
       <c r="A350" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B350" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C350" s="3">
-        <v>15</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C350" s="1"/>
       <c r="D350" s="3"/>
       <c r="E350" s="3"/>
-      <c r="F350" s="3"/>
+      <c r="F350" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="G350" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="351" spans="1:7" ht="15.75" thickBot="1">
       <c r="A351" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B351" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C351" s="1">
-        <v>20</v>
-      </c>
-      <c r="D351" s="3" t="s">
-        <v>159</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B351" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C351" s="3">
+        <v>15</v>
+      </c>
+      <c r="D351" s="3"/>
       <c r="E351" s="3"/>
       <c r="F351" s="3"/>
       <c r="G351" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="352" spans="1:7" ht="15.75" thickBot="1">
       <c r="A352" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B352" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C352" s="3">
-        <v>150</v>
-      </c>
-      <c r="D352" s="3"/>
-      <c r="E352" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C352" s="1">
+        <v>20</v>
+      </c>
+      <c r="D352" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E352" s="3"/>
       <c r="F352" s="3"/>
       <c r="G352" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="353" spans="1:7" ht="15.75" thickBot="1">
       <c r="A353" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B353" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C353" s="3">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="D353" s="3"/>
       <c r="E353" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F353" s="3" t="s">
+      <c r="F353" s="3"/>
+      <c r="G353" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A354" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B354" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C354" s="3">
+        <v>15</v>
+      </c>
+      <c r="D354" s="3"/>
+      <c r="E354" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F354" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G353" s="3" t="s">
+      <c r="G354" s="3" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="354" spans="1:7">
-      <c r="C354" s="5" t="s">
+    <row r="355" spans="1:7">
+      <c r="C355" s="5" t="s">
         <v>346</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="220">
+    <mergeCell ref="B343:G343"/>
+    <mergeCell ref="B344:G344"/>
+    <mergeCell ref="A345:G345"/>
+    <mergeCell ref="A346:A347"/>
+    <mergeCell ref="B346:B347"/>
+    <mergeCell ref="C346:C347"/>
+    <mergeCell ref="D346:D347"/>
+    <mergeCell ref="E346:E347"/>
+    <mergeCell ref="F346:F347"/>
+    <mergeCell ref="G346:G347"/>
+    <mergeCell ref="B333:G333"/>
+    <mergeCell ref="B334:G334"/>
+    <mergeCell ref="A335:G335"/>
+    <mergeCell ref="A336:A337"/>
+    <mergeCell ref="B336:B337"/>
+    <mergeCell ref="C336:C337"/>
+    <mergeCell ref="D336:D337"/>
+    <mergeCell ref="E336:E337"/>
+    <mergeCell ref="F336:F337"/>
+    <mergeCell ref="G336:G337"/>
+    <mergeCell ref="B305:G305"/>
+    <mergeCell ref="B306:G306"/>
+    <mergeCell ref="A307:G307"/>
+    <mergeCell ref="A308:A309"/>
+    <mergeCell ref="B308:B309"/>
+    <mergeCell ref="C308:C309"/>
+    <mergeCell ref="D308:D309"/>
+    <mergeCell ref="E308:E309"/>
+    <mergeCell ref="F308:F309"/>
+    <mergeCell ref="G308:G309"/>
+    <mergeCell ref="B287:G287"/>
+    <mergeCell ref="B288:G288"/>
+    <mergeCell ref="A289:G289"/>
+    <mergeCell ref="A290:A291"/>
+    <mergeCell ref="B290:B291"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="D290:D291"/>
+    <mergeCell ref="E290:E291"/>
+    <mergeCell ref="F290:F291"/>
+    <mergeCell ref="G290:G291"/>
+    <mergeCell ref="B268:G268"/>
+    <mergeCell ref="B269:G269"/>
+    <mergeCell ref="A270:G270"/>
+    <mergeCell ref="A271:A272"/>
+    <mergeCell ref="B271:B272"/>
+    <mergeCell ref="C271:C272"/>
+    <mergeCell ref="D271:D272"/>
+    <mergeCell ref="E271:E272"/>
+    <mergeCell ref="F271:F272"/>
+    <mergeCell ref="G271:G272"/>
+    <mergeCell ref="B255:G255"/>
+    <mergeCell ref="B256:G256"/>
+    <mergeCell ref="A257:G257"/>
+    <mergeCell ref="A258:A259"/>
+    <mergeCell ref="B258:B259"/>
+    <mergeCell ref="C258:C259"/>
+    <mergeCell ref="D258:D259"/>
+    <mergeCell ref="E258:E259"/>
+    <mergeCell ref="F258:F259"/>
+    <mergeCell ref="G258:G259"/>
+    <mergeCell ref="B244:G244"/>
+    <mergeCell ref="B245:G245"/>
+    <mergeCell ref="A246:G246"/>
+    <mergeCell ref="A247:A248"/>
+    <mergeCell ref="B247:B248"/>
+    <mergeCell ref="C247:C248"/>
+    <mergeCell ref="D247:D248"/>
+    <mergeCell ref="E247:E248"/>
+    <mergeCell ref="F247:F248"/>
+    <mergeCell ref="G247:G248"/>
+    <mergeCell ref="B233:G233"/>
+    <mergeCell ref="B234:G234"/>
+    <mergeCell ref="A235:G235"/>
+    <mergeCell ref="A236:A237"/>
+    <mergeCell ref="B236:B237"/>
+    <mergeCell ref="C236:C237"/>
+    <mergeCell ref="D236:D237"/>
+    <mergeCell ref="E236:E237"/>
+    <mergeCell ref="F236:F237"/>
+    <mergeCell ref="G236:G237"/>
+    <mergeCell ref="B186:G186"/>
+    <mergeCell ref="B187:G187"/>
+    <mergeCell ref="A188:G188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="B189:B190"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="E189:E190"/>
+    <mergeCell ref="F189:F190"/>
+    <mergeCell ref="G189:G190"/>
+    <mergeCell ref="B147:G147"/>
+    <mergeCell ref="B148:G148"/>
+    <mergeCell ref="A149:G149"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="D150:D151"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="F150:F151"/>
+    <mergeCell ref="G150:G151"/>
+    <mergeCell ref="B139:G139"/>
+    <mergeCell ref="B140:G140"/>
+    <mergeCell ref="A141:G141"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="E142:E143"/>
+    <mergeCell ref="F142:F143"/>
+    <mergeCell ref="G142:G143"/>
+    <mergeCell ref="B121:G121"/>
+    <mergeCell ref="B122:G122"/>
+    <mergeCell ref="A123:G123"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B106:G106"/>
+    <mergeCell ref="A107:G107"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="B90:G90"/>
+    <mergeCell ref="B91:G91"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="G93:G94"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="B80:G80"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
     <mergeCell ref="B58:G58"/>
     <mergeCell ref="B59:G59"/>
     <mergeCell ref="A60:G60"/>
@@ -12865,216 +13104,6 @@
     <mergeCell ref="E61:E62"/>
     <mergeCell ref="F61:F62"/>
     <mergeCell ref="G61:G62"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="B79:G79"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="B90:G90"/>
-    <mergeCell ref="B91:G91"/>
-    <mergeCell ref="A92:G92"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="G93:G94"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B106:G106"/>
-    <mergeCell ref="A107:G107"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="B121:G121"/>
-    <mergeCell ref="B122:G122"/>
-    <mergeCell ref="A123:G123"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="G124:G125"/>
-    <mergeCell ref="B139:G139"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="A141:G141"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="E142:E143"/>
-    <mergeCell ref="F142:F143"/>
-    <mergeCell ref="G142:G143"/>
-    <mergeCell ref="B147:G147"/>
-    <mergeCell ref="B148:G148"/>
-    <mergeCell ref="A149:G149"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="D150:D151"/>
-    <mergeCell ref="E150:E151"/>
-    <mergeCell ref="F150:F151"/>
-    <mergeCell ref="G150:G151"/>
-    <mergeCell ref="B186:G186"/>
-    <mergeCell ref="B187:G187"/>
-    <mergeCell ref="A188:G188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="B189:B190"/>
-    <mergeCell ref="C189:C190"/>
-    <mergeCell ref="D189:D190"/>
-    <mergeCell ref="E189:E190"/>
-    <mergeCell ref="F189:F190"/>
-    <mergeCell ref="G189:G190"/>
-    <mergeCell ref="B233:G233"/>
-    <mergeCell ref="B234:G234"/>
-    <mergeCell ref="A235:G235"/>
-    <mergeCell ref="A236:A237"/>
-    <mergeCell ref="B236:B237"/>
-    <mergeCell ref="C236:C237"/>
-    <mergeCell ref="D236:D237"/>
-    <mergeCell ref="E236:E237"/>
-    <mergeCell ref="F236:F237"/>
-    <mergeCell ref="G236:G237"/>
-    <mergeCell ref="B244:G244"/>
-    <mergeCell ref="B245:G245"/>
-    <mergeCell ref="A246:G246"/>
-    <mergeCell ref="A247:A248"/>
-    <mergeCell ref="B247:B248"/>
-    <mergeCell ref="C247:C248"/>
-    <mergeCell ref="D247:D248"/>
-    <mergeCell ref="E247:E248"/>
-    <mergeCell ref="F247:F248"/>
-    <mergeCell ref="G247:G248"/>
-    <mergeCell ref="B255:G255"/>
-    <mergeCell ref="B256:G256"/>
-    <mergeCell ref="A257:G257"/>
-    <mergeCell ref="A258:A259"/>
-    <mergeCell ref="B258:B259"/>
-    <mergeCell ref="C258:C259"/>
-    <mergeCell ref="D258:D259"/>
-    <mergeCell ref="E258:E259"/>
-    <mergeCell ref="F258:F259"/>
-    <mergeCell ref="G258:G259"/>
-    <mergeCell ref="B268:G268"/>
-    <mergeCell ref="B269:G269"/>
-    <mergeCell ref="A270:G270"/>
-    <mergeCell ref="A271:A272"/>
-    <mergeCell ref="B271:B272"/>
-    <mergeCell ref="C271:C272"/>
-    <mergeCell ref="D271:D272"/>
-    <mergeCell ref="E271:E272"/>
-    <mergeCell ref="F271:F272"/>
-    <mergeCell ref="G271:G272"/>
-    <mergeCell ref="B286:G286"/>
-    <mergeCell ref="B287:G287"/>
-    <mergeCell ref="A288:G288"/>
-    <mergeCell ref="A289:A290"/>
-    <mergeCell ref="B289:B290"/>
-    <mergeCell ref="C289:C290"/>
-    <mergeCell ref="D289:D290"/>
-    <mergeCell ref="E289:E290"/>
-    <mergeCell ref="F289:F290"/>
-    <mergeCell ref="G289:G290"/>
-    <mergeCell ref="B304:G304"/>
-    <mergeCell ref="B305:G305"/>
-    <mergeCell ref="A306:G306"/>
-    <mergeCell ref="A307:A308"/>
-    <mergeCell ref="B307:B308"/>
-    <mergeCell ref="C307:C308"/>
-    <mergeCell ref="D307:D308"/>
-    <mergeCell ref="E307:E308"/>
-    <mergeCell ref="F307:F308"/>
-    <mergeCell ref="G307:G308"/>
-    <mergeCell ref="B332:G332"/>
-    <mergeCell ref="B333:G333"/>
-    <mergeCell ref="A334:G334"/>
-    <mergeCell ref="A335:A336"/>
-    <mergeCell ref="B335:B336"/>
-    <mergeCell ref="C335:C336"/>
-    <mergeCell ref="D335:D336"/>
-    <mergeCell ref="E335:E336"/>
-    <mergeCell ref="F335:F336"/>
-    <mergeCell ref="G335:G336"/>
-    <mergeCell ref="B342:G342"/>
-    <mergeCell ref="B343:G343"/>
-    <mergeCell ref="A344:G344"/>
-    <mergeCell ref="A345:A346"/>
-    <mergeCell ref="B345:B346"/>
-    <mergeCell ref="C345:C346"/>
-    <mergeCell ref="D345:D346"/>
-    <mergeCell ref="E345:E346"/>
-    <mergeCell ref="F345:F346"/>
-    <mergeCell ref="G345:G346"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Pronta Funcion Gestion Compras
</commit_message>
<xml_diff>
--- a/html/database/Diccionario de Datos.xlsx
+++ b/html/database/Diccionario de Datos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario de Datos - TABLAS" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="368">
   <si>
     <t>Nombre de la tabla</t>
   </si>
@@ -1628,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L243"/>
+  <dimension ref="A1:L244"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="A198" sqref="A198"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="L126" sqref="L126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25"/>
@@ -4319,55 +4319,65 @@
     </row>
     <row r="126" spans="1:12" ht="12" thickBot="1">
       <c r="A126" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C126" s="10">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D126" s="10"/>
       <c r="E126" s="10"/>
       <c r="F126" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G126" s="10">
-        <v>0</v>
+      <c r="G126" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="H126" s="10"/>
-      <c r="I126" s="10"/>
+      <c r="I126" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="J126" s="10"/>
       <c r="K126" s="10"/>
-      <c r="L126" s="10" t="s">
+      <c r="L126" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" ht="12" thickBot="1">
+      <c r="A127" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C127" s="10">
+        <v>1</v>
+      </c>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+      <c r="F127" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G127" s="10">
+        <v>0</v>
+      </c>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="J127" s="10"/>
+      <c r="K127" s="10"/>
+      <c r="L127" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="12" thickBot="1"/>
-    <row r="128" spans="1:12" ht="12" thickBot="1">
-      <c r="A128" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B128" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C128" s="13"/>
-      <c r="D128" s="13"/>
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
-      <c r="J128" s="13"/>
-      <c r="K128" s="13"/>
-      <c r="L128" s="14"/>
-    </row>
+    <row r="128" spans="1:12" ht="12" thickBot="1"/>
     <row r="129" spans="1:12" ht="12" thickBot="1">
       <c r="A129" s="8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="C129" s="13"/>
       <c r="D129" s="13"/>
@@ -4381,10 +4391,12 @@
       <c r="L129" s="14"/>
     </row>
     <row r="130" spans="1:12" ht="12" thickBot="1">
-      <c r="A130" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B130" s="13"/>
+      <c r="A130" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="C130" s="13"/>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
@@ -4397,116 +4409,104 @@
       <c r="L130" s="14"/>
     </row>
     <row r="131" spans="1:12" ht="12" thickBot="1">
-      <c r="A131" s="15" t="s">
+      <c r="A131" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131" s="13"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="13"/>
+      <c r="J131" s="13"/>
+      <c r="K131" s="13"/>
+      <c r="L131" s="14"/>
+    </row>
+    <row r="132" spans="1:12" ht="12" thickBot="1">
+      <c r="A132" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B131" s="15" t="s">
+      <c r="B132" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C132" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D131" s="15" t="s">
+      <c r="D132" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E131" s="15" t="s">
+      <c r="E132" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F131" s="15" t="s">
+      <c r="F132" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G131" s="15" t="s">
+      <c r="G132" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H131" s="17" t="s">
+      <c r="H132" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I131" s="15" t="s">
+      <c r="I132" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J131" s="12" t="s">
+      <c r="J132" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K131" s="14"/>
-      <c r="L131" s="15" t="s">
+      <c r="K132" s="14"/>
+      <c r="L132" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="12" thickBot="1">
-      <c r="A132" s="16"/>
-      <c r="B132" s="16"/>
-      <c r="C132" s="16"/>
-      <c r="D132" s="16"/>
-      <c r="E132" s="16"/>
-      <c r="F132" s="16"/>
-      <c r="G132" s="16"/>
-      <c r="H132" s="18"/>
-      <c r="I132" s="16"/>
-      <c r="J132" s="8" t="s">
+    <row r="133" spans="1:12" ht="12" thickBot="1">
+      <c r="A133" s="16"/>
+      <c r="B133" s="16"/>
+      <c r="C133" s="16"/>
+      <c r="D133" s="16"/>
+      <c r="E133" s="16"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="18"/>
+      <c r="I133" s="16"/>
+      <c r="J133" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K132" s="8" t="s">
+      <c r="K133" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L132" s="16"/>
-    </row>
-    <row r="133" spans="1:12" ht="12" thickBot="1">
-      <c r="A133" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B133" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C133" s="10"/>
-      <c r="D133" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E133" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F133" s="10"/>
-      <c r="G133" s="10"/>
-      <c r="H133" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I133" s="10"/>
-      <c r="J133" s="10"/>
-      <c r="K133" s="10"/>
-      <c r="L133" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="L133" s="16"/>
     </row>
     <row r="134" spans="1:12" ht="12" thickBot="1">
       <c r="A134" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B134" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C134" s="8">
-        <v>20</v>
-      </c>
-      <c r="D134" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E134" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C134" s="10"/>
+      <c r="D134" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E134" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F134" s="10"/>
       <c r="G134" s="10"/>
-      <c r="H134" s="10"/>
+      <c r="H134" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I134" s="10"/>
-      <c r="J134" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="K134" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L134" s="8" t="s">
-        <v>103</v>
+      <c r="J134" s="10"/>
+      <c r="K134" s="10"/>
+      <c r="L134" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="135" spans="1:12" ht="12" thickBot="1">
-      <c r="A135" s="8" t="s">
-        <v>59</v>
+      <c r="A135" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="B135" s="8" t="s">
         <v>102</v>
@@ -4523,7 +4523,7 @@
       <c r="H135" s="10"/>
       <c r="I135" s="10"/>
       <c r="J135" s="10" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="K135" s="10" t="s">
         <v>14</v>
@@ -4533,8 +4533,8 @@
       </c>
     </row>
     <row r="136" spans="1:12" ht="12" thickBot="1">
-      <c r="A136" s="10" t="s">
-        <v>60</v>
+      <c r="A136" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B136" s="8" t="s">
         <v>102</v>
@@ -4551,7 +4551,7 @@
       <c r="H136" s="10"/>
       <c r="I136" s="10"/>
       <c r="J136" s="10" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="K136" s="10" t="s">
         <v>14</v>
@@ -4561,50 +4561,58 @@
       </c>
     </row>
     <row r="137" spans="1:12" ht="12" thickBot="1">
-      <c r="A137" s="8" t="s">
-        <v>51</v>
+      <c r="A137" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
-      <c r="F137" s="8"/>
-      <c r="G137" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H137" s="8"/>
-      <c r="I137" s="8"/>
-      <c r="J137" s="8"/>
-      <c r="K137" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="C137" s="8">
+        <v>20</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E137" s="10"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="10"/>
+      <c r="J137" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K137" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="L137" s="8" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="138" spans="1:12" ht="12" thickBot="1">
       <c r="A138" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
       <c r="E138" s="8"/>
       <c r="F138" s="8"/>
-      <c r="G138" s="8"/>
+      <c r="G138" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="H138" s="8"/>
       <c r="I138" s="8"/>
       <c r="J138" s="8"/>
       <c r="K138" s="8"/>
       <c r="L138" s="8" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="139" spans="1:12" ht="12" thickBot="1">
       <c r="A139" s="8" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>80</v>
@@ -4612,28 +4620,24 @@
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
       <c r="E139" s="8"/>
-      <c r="F139" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="F139" s="8"/>
       <c r="G139" s="8"/>
       <c r="H139" s="8"/>
       <c r="I139" s="8"/>
       <c r="J139" s="8"/>
       <c r="K139" s="8"/>
       <c r="L139" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="12" thickBot="1">
       <c r="A140" s="8" t="s">
-        <v>28</v>
+        <v>132</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C140" s="8">
-        <v>15</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C140" s="8"/>
       <c r="D140" s="8"/>
       <c r="E140" s="8"/>
       <c r="F140" s="8" t="s">
@@ -4641,84 +4645,90 @@
       </c>
       <c r="G140" s="8"/>
       <c r="H140" s="8"/>
-      <c r="I140" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="I140" s="8"/>
       <c r="J140" s="8"/>
       <c r="K140" s="8"/>
       <c r="L140" s="8" t="s">
-        <v>359</v>
+        <v>134</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="12" thickBot="1">
       <c r="A141" s="8" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C141" s="8"/>
+        <v>79</v>
+      </c>
+      <c r="C141" s="8">
+        <v>15</v>
+      </c>
       <c r="D141" s="8"/>
       <c r="E141" s="8"/>
-      <c r="F141" s="8"/>
+      <c r="F141" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="G141" s="8"/>
       <c r="H141" s="8"/>
-      <c r="I141" s="8"/>
+      <c r="I141" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="J141" s="8"/>
       <c r="K141" s="8"/>
-      <c r="L141" s="8"/>
+      <c r="L141" s="8" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="142" spans="1:12" ht="12" thickBot="1">
-      <c r="A142" s="10" t="s">
+      <c r="A142" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+      <c r="F142" s="8"/>
+      <c r="G142" s="8"/>
+      <c r="H142" s="8"/>
+      <c r="I142" s="8"/>
+      <c r="J142" s="8"/>
+      <c r="K142" s="8"/>
+      <c r="L142" s="8"/>
+    </row>
+    <row r="143" spans="1:12" ht="12" thickBot="1">
+      <c r="A143" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B142" s="10" t="s">
+      <c r="B143" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C142" s="10">
+      <c r="C143" s="10">
         <v>1</v>
       </c>
-      <c r="D142" s="10"/>
-      <c r="E142" s="10"/>
-      <c r="F142" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G142" s="10">
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G143" s="10">
         <v>0</v>
       </c>
-      <c r="H142" s="10"/>
-      <c r="I142" s="10"/>
-      <c r="J142" s="10"/>
-      <c r="K142" s="10"/>
-      <c r="L142" s="10" t="s">
+      <c r="H143" s="10"/>
+      <c r="I143" s="10"/>
+      <c r="J143" s="10"/>
+      <c r="K143" s="10"/>
+      <c r="L143" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="12" thickBot="1"/>
-    <row r="144" spans="1:12" ht="12" thickBot="1">
-      <c r="A144" s="8" t="s">
+    <row r="144" spans="1:12" ht="12" thickBot="1"/>
+    <row r="145" spans="1:12" ht="12" thickBot="1">
+      <c r="A145" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B144" s="12" t="s">
+      <c r="B145" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="C144" s="13"/>
-      <c r="D144" s="13"/>
-      <c r="E144" s="13"/>
-      <c r="F144" s="13"/>
-      <c r="G144" s="13"/>
-      <c r="H144" s="13"/>
-      <c r="I144" s="13"/>
-      <c r="J144" s="13"/>
-      <c r="K144" s="13"/>
-      <c r="L144" s="14"/>
-    </row>
-    <row r="145" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A145" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B145" s="12" t="s">
-        <v>136</v>
       </c>
       <c r="C145" s="13"/>
       <c r="D145" s="13"/>
@@ -4731,11 +4741,13 @@
       <c r="K145" s="13"/>
       <c r="L145" s="14"/>
     </row>
-    <row r="146" spans="1:12" ht="12" thickBot="1">
-      <c r="A146" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B146" s="13"/>
+    <row r="146" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A146" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B146" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="C146" s="13"/>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
@@ -4748,116 +4760,104 @@
       <c r="L146" s="14"/>
     </row>
     <row r="147" spans="1:12" ht="12" thickBot="1">
-      <c r="A147" s="15" t="s">
+      <c r="A147" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B147" s="13"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="13"/>
+      <c r="G147" s="13"/>
+      <c r="H147" s="13"/>
+      <c r="I147" s="13"/>
+      <c r="J147" s="13"/>
+      <c r="K147" s="13"/>
+      <c r="L147" s="14"/>
+    </row>
+    <row r="148" spans="1:12" ht="12" thickBot="1">
+      <c r="A148" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B147" s="15" t="s">
+      <c r="B148" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C147" s="15" t="s">
+      <c r="C148" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D147" s="15" t="s">
+      <c r="D148" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E147" s="15" t="s">
+      <c r="E148" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F147" s="15" t="s">
+      <c r="F148" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G147" s="15" t="s">
+      <c r="G148" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H147" s="17" t="s">
+      <c r="H148" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I147" s="15" t="s">
+      <c r="I148" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J147" s="12" t="s">
+      <c r="J148" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K147" s="14"/>
-      <c r="L147" s="15" t="s">
+      <c r="K148" s="14"/>
+      <c r="L148" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="12" thickBot="1">
-      <c r="A148" s="16"/>
-      <c r="B148" s="16"/>
-      <c r="C148" s="16"/>
-      <c r="D148" s="16"/>
-      <c r="E148" s="16"/>
-      <c r="F148" s="16"/>
-      <c r="G148" s="16"/>
-      <c r="H148" s="18"/>
-      <c r="I148" s="16"/>
-      <c r="J148" s="8" t="s">
+    <row r="149" spans="1:12" ht="12" thickBot="1">
+      <c r="A149" s="16"/>
+      <c r="B149" s="16"/>
+      <c r="C149" s="16"/>
+      <c r="D149" s="16"/>
+      <c r="E149" s="16"/>
+      <c r="F149" s="16"/>
+      <c r="G149" s="16"/>
+      <c r="H149" s="18"/>
+      <c r="I149" s="16"/>
+      <c r="J149" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K148" s="8" t="s">
+      <c r="K149" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L148" s="16"/>
-    </row>
-    <row r="149" spans="1:12" ht="12" thickBot="1">
-      <c r="A149" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B149" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C149" s="10"/>
-      <c r="D149" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E149" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F149" s="10"/>
-      <c r="G149" s="10"/>
-      <c r="H149" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I149" s="10"/>
-      <c r="J149" s="10"/>
-      <c r="K149" s="10"/>
-      <c r="L149" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="L149" s="16"/>
     </row>
     <row r="150" spans="1:12" ht="12" thickBot="1">
       <c r="A150" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B150" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C150" s="8">
-        <v>20</v>
-      </c>
-      <c r="D150" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E150" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C150" s="10"/>
+      <c r="D150" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E150" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F150" s="10"/>
       <c r="G150" s="10"/>
-      <c r="H150" s="10"/>
+      <c r="H150" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I150" s="10"/>
-      <c r="J150" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="K150" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L150" s="8" t="s">
-        <v>103</v>
+      <c r="J150" s="10"/>
+      <c r="K150" s="10"/>
+      <c r="L150" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="12" thickBot="1">
-      <c r="A151" s="8" t="s">
-        <v>59</v>
+      <c r="A151" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>102</v>
@@ -4874,7 +4874,7 @@
       <c r="H151" s="10"/>
       <c r="I151" s="10"/>
       <c r="J151" s="10" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="K151" s="10" t="s">
         <v>14</v>
@@ -4884,8 +4884,8 @@
       </c>
     </row>
     <row r="152" spans="1:12" ht="12" thickBot="1">
-      <c r="A152" s="10" t="s">
-        <v>60</v>
+      <c r="A152" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>102</v>
@@ -4902,7 +4902,7 @@
       <c r="H152" s="10"/>
       <c r="I152" s="10"/>
       <c r="J152" s="10" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="K152" s="10" t="s">
         <v>14</v>
@@ -4912,55 +4912,61 @@
       </c>
     </row>
     <row r="153" spans="1:12" ht="12" thickBot="1">
-      <c r="A153" s="8" t="s">
-        <v>47</v>
+      <c r="A153" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
-      <c r="E153" s="8"/>
-      <c r="F153" s="8"/>
-      <c r="G153" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H153" s="8"/>
-      <c r="I153" s="8"/>
-      <c r="J153" s="8"/>
-      <c r="K153" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="C153" s="8">
+        <v>20</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E153" s="10"/>
+      <c r="F153" s="10"/>
+      <c r="G153" s="10"/>
+      <c r="H153" s="10"/>
+      <c r="I153" s="10"/>
+      <c r="J153" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K153" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="L153" s="8" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="154" spans="1:12" ht="12" thickBot="1">
       <c r="A154" s="8" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
       <c r="E154" s="8"/>
       <c r="F154" s="8"/>
-      <c r="G154" s="8"/>
+      <c r="G154" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="H154" s="8"/>
-      <c r="I154" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="I154" s="8"/>
       <c r="J154" s="8"/>
       <c r="K154" s="8"/>
       <c r="L154" s="8" t="s">
-        <v>360</v>
+        <v>116</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="12" thickBot="1">
       <c r="A155" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
@@ -4968,64 +4974,68 @@
       <c r="F155" s="8"/>
       <c r="G155" s="8"/>
       <c r="H155" s="8"/>
-      <c r="I155" s="8"/>
+      <c r="I155" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="J155" s="8"/>
       <c r="K155" s="8"/>
       <c r="L155" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" ht="12" thickBot="1">
+      <c r="A156" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
+      <c r="F156" s="8"/>
+      <c r="G156" s="8"/>
+      <c r="H156" s="8"/>
+      <c r="I156" s="8"/>
+      <c r="J156" s="8"/>
+      <c r="K156" s="8"/>
+      <c r="L156" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="12" thickBot="1">
-      <c r="A156" s="10" t="s">
+    <row r="157" spans="1:12" ht="12" thickBot="1">
+      <c r="A157" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B156" s="10" t="s">
+      <c r="B157" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C156" s="10">
+      <c r="C157" s="10">
         <v>1</v>
       </c>
-      <c r="D156" s="10"/>
-      <c r="E156" s="10"/>
-      <c r="F156" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G156" s="10">
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
+      <c r="F157" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G157" s="10">
         <v>0</v>
       </c>
-      <c r="H156" s="10"/>
-      <c r="I156" s="10"/>
-      <c r="J156" s="10"/>
-      <c r="K156" s="10"/>
-      <c r="L156" s="10" t="s">
+      <c r="H157" s="10"/>
+      <c r="I157" s="10"/>
+      <c r="J157" s="10"/>
+      <c r="K157" s="10"/>
+      <c r="L157" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="12" thickBot="1"/>
-    <row r="158" spans="1:12" ht="12" thickBot="1">
-      <c r="A158" s="8" t="s">
+    <row r="158" spans="1:12" ht="12" thickBot="1"/>
+    <row r="159" spans="1:12" ht="12" thickBot="1">
+      <c r="A159" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B158" s="12" t="s">
+      <c r="B159" s="12" t="s">
         <v>135</v>
-      </c>
-      <c r="C158" s="13"/>
-      <c r="D158" s="13"/>
-      <c r="E158" s="13"/>
-      <c r="F158" s="13"/>
-      <c r="G158" s="13"/>
-      <c r="H158" s="13"/>
-      <c r="I158" s="13"/>
-      <c r="J158" s="13"/>
-      <c r="K158" s="13"/>
-      <c r="L158" s="14"/>
-    </row>
-    <row r="159" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A159" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B159" s="12" t="s">
-        <v>140</v>
       </c>
       <c r="C159" s="13"/>
       <c r="D159" s="13"/>
@@ -5038,11 +5048,13 @@
       <c r="K159" s="13"/>
       <c r="L159" s="14"/>
     </row>
-    <row r="160" spans="1:12" ht="12" thickBot="1">
-      <c r="A160" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B160" s="13"/>
+    <row r="160" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A160" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B160" s="12" t="s">
+        <v>140</v>
+      </c>
       <c r="C160" s="13"/>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
@@ -5055,116 +5067,104 @@
       <c r="L160" s="14"/>
     </row>
     <row r="161" spans="1:12" ht="12" thickBot="1">
-      <c r="A161" s="15" t="s">
+      <c r="A161" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B161" s="13"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="13"/>
+      <c r="H161" s="13"/>
+      <c r="I161" s="13"/>
+      <c r="J161" s="13"/>
+      <c r="K161" s="13"/>
+      <c r="L161" s="14"/>
+    </row>
+    <row r="162" spans="1:12" ht="12" thickBot="1">
+      <c r="A162" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B161" s="15" t="s">
+      <c r="B162" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C161" s="15" t="s">
+      <c r="C162" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D161" s="15" t="s">
+      <c r="D162" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E161" s="15" t="s">
+      <c r="E162" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F161" s="15" t="s">
+      <c r="F162" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G161" s="15" t="s">
+      <c r="G162" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H161" s="17" t="s">
+      <c r="H162" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I161" s="15" t="s">
+      <c r="I162" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J161" s="12" t="s">
+      <c r="J162" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K161" s="14"/>
-      <c r="L161" s="15" t="s">
+      <c r="K162" s="14"/>
+      <c r="L162" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="12" thickBot="1">
-      <c r="A162" s="16"/>
-      <c r="B162" s="16"/>
-      <c r="C162" s="16"/>
-      <c r="D162" s="16"/>
-      <c r="E162" s="16"/>
-      <c r="F162" s="16"/>
-      <c r="G162" s="16"/>
-      <c r="H162" s="18"/>
-      <c r="I162" s="16"/>
-      <c r="J162" s="8" t="s">
+    <row r="163" spans="1:12" ht="12" thickBot="1">
+      <c r="A163" s="16"/>
+      <c r="B163" s="16"/>
+      <c r="C163" s="16"/>
+      <c r="D163" s="16"/>
+      <c r="E163" s="16"/>
+      <c r="F163" s="16"/>
+      <c r="G163" s="16"/>
+      <c r="H163" s="18"/>
+      <c r="I163" s="16"/>
+      <c r="J163" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K162" s="8" t="s">
+      <c r="K163" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L162" s="16"/>
-    </row>
-    <row r="163" spans="1:12" ht="12" thickBot="1">
-      <c r="A163" s="10" t="s">
+      <c r="L163" s="16"/>
+    </row>
+    <row r="164" spans="1:12" ht="12" thickBot="1">
+      <c r="A164" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B163" s="10" t="s">
+      <c r="B164" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C163" s="10"/>
-      <c r="D163" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E163" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F163" s="10"/>
-      <c r="G163" s="10"/>
-      <c r="H163" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I163" s="10"/>
-      <c r="J163" s="10"/>
-      <c r="K163" s="10"/>
-      <c r="L163" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="164" spans="1:12" ht="12" thickBot="1">
-      <c r="A164" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B164" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C164" s="8">
-        <v>20</v>
-      </c>
-      <c r="D164" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E164" s="10"/>
+      <c r="C164" s="10"/>
+      <c r="D164" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E164" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F164" s="10"/>
       <c r="G164" s="10"/>
-      <c r="H164" s="10"/>
+      <c r="H164" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I164" s="10"/>
-      <c r="J164" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K164" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L164" s="8" t="s">
-        <v>103</v>
+      <c r="J164" s="10"/>
+      <c r="K164" s="10"/>
+      <c r="L164" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="12" thickBot="1">
-      <c r="A165" s="10" t="s">
-        <v>60</v>
+      <c r="A165" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>102</v>
@@ -5181,7 +5181,7 @@
       <c r="H165" s="10"/>
       <c r="I165" s="10"/>
       <c r="J165" s="10" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="K165" s="10" t="s">
         <v>14</v>
@@ -5191,164 +5191,174 @@
       </c>
     </row>
     <row r="166" spans="1:12" ht="12" thickBot="1">
-      <c r="A166" s="8" t="s">
-        <v>65</v>
+      <c r="A166" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C166" s="8">
-        <v>150</v>
-      </c>
-      <c r="D166" s="8"/>
-      <c r="E166" s="8"/>
-      <c r="F166" s="8"/>
-      <c r="G166" s="8"/>
-      <c r="H166" s="8"/>
-      <c r="I166" s="8"/>
-      <c r="J166" s="8"/>
-      <c r="K166" s="8"/>
-      <c r="L166" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="D166" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E166" s="10"/>
+      <c r="F166" s="10"/>
+      <c r="G166" s="10"/>
+      <c r="H166" s="10"/>
+      <c r="I166" s="10"/>
+      <c r="J166" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K166" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L166" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="167" spans="1:12" ht="12" thickBot="1">
       <c r="A167" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C167" s="8"/>
+        <v>79</v>
+      </c>
+      <c r="C167" s="8">
+        <v>150</v>
+      </c>
       <c r="D167" s="8"/>
       <c r="E167" s="8"/>
       <c r="F167" s="8"/>
-      <c r="G167" s="8" t="s">
-        <v>115</v>
-      </c>
+      <c r="G167" s="8"/>
       <c r="H167" s="8"/>
       <c r="I167" s="8"/>
       <c r="J167" s="8"/>
       <c r="K167" s="8"/>
-      <c r="L167" s="8" t="s">
-        <v>139</v>
-      </c>
+      <c r="L167" s="8"/>
     </row>
     <row r="168" spans="1:12" ht="12" thickBot="1">
       <c r="A168" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C168" s="8">
-        <v>150</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C168" s="8"/>
       <c r="D168" s="8"/>
       <c r="E168" s="8"/>
-      <c r="F168" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G168" s="8"/>
+      <c r="F168" s="8"/>
+      <c r="G168" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="H168" s="8"/>
       <c r="I168" s="8"/>
       <c r="J168" s="8"/>
       <c r="K168" s="8"/>
-      <c r="L168" s="8"/>
+      <c r="L168" s="8" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="169" spans="1:12" ht="12" thickBot="1">
       <c r="A169" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C169" s="8"/>
+        <v>79</v>
+      </c>
+      <c r="C169" s="8">
+        <v>150</v>
+      </c>
       <c r="D169" s="8"/>
       <c r="E169" s="8"/>
-      <c r="F169" s="8"/>
+      <c r="F169" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="G169" s="8"/>
       <c r="H169" s="8"/>
       <c r="I169" s="8"/>
       <c r="J169" s="8"/>
       <c r="K169" s="8"/>
-      <c r="L169" s="8" t="s">
-        <v>88</v>
-      </c>
+      <c r="L169" s="8"/>
     </row>
     <row r="170" spans="1:12" ht="12" thickBot="1">
       <c r="A170" s="8" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C170" s="8">
-        <v>15</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C170" s="8"/>
       <c r="D170" s="8"/>
       <c r="E170" s="8"/>
       <c r="F170" s="8"/>
-      <c r="G170" s="8" t="s">
-        <v>138</v>
-      </c>
+      <c r="G170" s="8"/>
       <c r="H170" s="8"/>
       <c r="I170" s="8"/>
       <c r="J170" s="8"/>
       <c r="K170" s="8"/>
       <c r="L170" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" ht="12" thickBot="1">
+      <c r="A171" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C171" s="8">
+        <v>15</v>
+      </c>
+      <c r="D171" s="8"/>
+      <c r="E171" s="8"/>
+      <c r="F171" s="8"/>
+      <c r="G171" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H171" s="8"/>
+      <c r="I171" s="8"/>
+      <c r="J171" s="8"/>
+      <c r="K171" s="8"/>
+      <c r="L171" s="8" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="171" spans="1:12" ht="12" thickBot="1">
-      <c r="A171" s="10" t="s">
+    <row r="172" spans="1:12" ht="12" thickBot="1">
+      <c r="A172" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B171" s="10" t="s">
+      <c r="B172" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C171" s="10">
+      <c r="C172" s="10">
         <v>1</v>
       </c>
-      <c r="D171" s="10"/>
-      <c r="E171" s="10"/>
-      <c r="F171" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G171" s="10">
+      <c r="D172" s="10"/>
+      <c r="E172" s="10"/>
+      <c r="F172" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G172" s="10">
         <v>0</v>
       </c>
-      <c r="H171" s="10"/>
-      <c r="I171" s="10"/>
-      <c r="J171" s="10"/>
-      <c r="K171" s="10"/>
-      <c r="L171" s="10" t="s">
+      <c r="H172" s="10"/>
+      <c r="I172" s="10"/>
+      <c r="J172" s="10"/>
+      <c r="K172" s="10"/>
+      <c r="L172" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="12" thickBot="1"/>
-    <row r="173" spans="1:12" ht="12" thickBot="1">
-      <c r="A173" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B173" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C173" s="13"/>
-      <c r="D173" s="13"/>
-      <c r="E173" s="13"/>
-      <c r="F173" s="13"/>
-      <c r="G173" s="13"/>
-      <c r="H173" s="13"/>
-      <c r="I173" s="13"/>
-      <c r="J173" s="13"/>
-      <c r="K173" s="13"/>
-      <c r="L173" s="14"/>
-    </row>
+    <row r="173" spans="1:12" ht="12" thickBot="1"/>
     <row r="174" spans="1:12" ht="12" thickBot="1">
       <c r="A174" s="8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B174" s="12" t="s">
-        <v>141</v>
+        <v>69</v>
       </c>
       <c r="C174" s="13"/>
       <c r="D174" s="13"/>
@@ -5362,10 +5372,12 @@
       <c r="L174" s="14"/>
     </row>
     <row r="175" spans="1:12" ht="12" thickBot="1">
-      <c r="A175" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B175" s="13"/>
+      <c r="A175" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B175" s="12" t="s">
+        <v>141</v>
+      </c>
       <c r="C175" s="13"/>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
@@ -5378,116 +5390,104 @@
       <c r="L175" s="14"/>
     </row>
     <row r="176" spans="1:12" ht="12" thickBot="1">
-      <c r="A176" s="15" t="s">
+      <c r="A176" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B176" s="13"/>
+      <c r="C176" s="13"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
+      <c r="F176" s="13"/>
+      <c r="G176" s="13"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="13"/>
+      <c r="J176" s="13"/>
+      <c r="K176" s="13"/>
+      <c r="L176" s="14"/>
+    </row>
+    <row r="177" spans="1:12" ht="12" thickBot="1">
+      <c r="A177" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B176" s="15" t="s">
+      <c r="B177" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C176" s="15" t="s">
+      <c r="C177" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D176" s="15" t="s">
+      <c r="D177" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E176" s="15" t="s">
+      <c r="E177" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F176" s="15" t="s">
+      <c r="F177" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G176" s="15" t="s">
+      <c r="G177" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H176" s="17" t="s">
+      <c r="H177" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I176" s="15" t="s">
+      <c r="I177" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J176" s="12" t="s">
+      <c r="J177" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K176" s="14"/>
-      <c r="L176" s="15" t="s">
+      <c r="K177" s="14"/>
+      <c r="L177" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:12" ht="12" thickBot="1">
-      <c r="A177" s="16"/>
-      <c r="B177" s="16"/>
-      <c r="C177" s="16"/>
-      <c r="D177" s="16"/>
-      <c r="E177" s="16"/>
-      <c r="F177" s="16"/>
-      <c r="G177" s="16"/>
-      <c r="H177" s="18"/>
-      <c r="I177" s="16"/>
-      <c r="J177" s="8" t="s">
+    <row r="178" spans="1:12" ht="12" thickBot="1">
+      <c r="A178" s="16"/>
+      <c r="B178" s="16"/>
+      <c r="C178" s="16"/>
+      <c r="D178" s="16"/>
+      <c r="E178" s="16"/>
+      <c r="F178" s="16"/>
+      <c r="G178" s="16"/>
+      <c r="H178" s="18"/>
+      <c r="I178" s="16"/>
+      <c r="J178" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K177" s="8" t="s">
+      <c r="K178" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L177" s="16"/>
-    </row>
-    <row r="178" spans="1:12" ht="12" thickBot="1">
-      <c r="A178" s="10" t="s">
+      <c r="L178" s="16"/>
+    </row>
+    <row r="179" spans="1:12" ht="12" thickBot="1">
+      <c r="A179" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B178" s="10" t="s">
+      <c r="B179" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C178" s="10"/>
-      <c r="D178" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E178" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F178" s="10"/>
-      <c r="G178" s="10"/>
-      <c r="H178" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I178" s="10"/>
-      <c r="J178" s="10"/>
-      <c r="K178" s="10"/>
-      <c r="L178" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="179" spans="1:12" ht="12" thickBot="1">
-      <c r="A179" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B179" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C179" s="8">
-        <v>20</v>
-      </c>
-      <c r="D179" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E179" s="10"/>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E179" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F179" s="10"/>
       <c r="G179" s="10"/>
-      <c r="H179" s="10"/>
+      <c r="H179" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I179" s="10"/>
-      <c r="J179" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K179" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L179" s="8" t="s">
-        <v>103</v>
+      <c r="J179" s="10"/>
+      <c r="K179" s="10"/>
+      <c r="L179" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="12" thickBot="1">
       <c r="A180" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B180" s="8" t="s">
         <v>102</v>
@@ -5515,151 +5515,161 @@
     </row>
     <row r="181" spans="1:12" ht="12" thickBot="1">
       <c r="A181" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B181" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C181" s="10">
-        <v>15</v>
-      </c>
-      <c r="D181" s="10"/>
+        <v>143</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C181" s="8">
+        <v>20</v>
+      </c>
+      <c r="D181" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="E181" s="10"/>
-      <c r="F181" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G181" s="10" t="s">
-        <v>144</v>
-      </c>
+      <c r="F181" s="10"/>
+      <c r="G181" s="10"/>
       <c r="H181" s="10"/>
-      <c r="I181" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J181" s="8"/>
-      <c r="K181" s="8"/>
+      <c r="I181" s="10"/>
+      <c r="J181" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K181" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="L181" s="8" t="s">
-        <v>362</v>
+        <v>103</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="12" thickBot="1">
       <c r="A182" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B182" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C182" s="8"/>
-      <c r="D182" s="8"/>
-      <c r="E182" s="8"/>
-      <c r="F182" s="8"/>
-      <c r="G182" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H182" s="8"/>
-      <c r="I182" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="B182" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C182" s="10">
+        <v>15</v>
+      </c>
+      <c r="D182" s="10"/>
+      <c r="E182" s="10"/>
+      <c r="F182" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G182" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H182" s="10"/>
+      <c r="I182" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="J182" s="8"/>
       <c r="K182" s="8"/>
       <c r="L182" s="8" t="s">
-        <v>145</v>
+        <v>362</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="12" thickBot="1">
       <c r="A183" s="8" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C183" s="8">
-        <v>1</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C183" s="8"/>
       <c r="D183" s="8"/>
       <c r="E183" s="8"/>
-      <c r="F183" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G183" s="8">
-        <v>0</v>
+      <c r="F183" s="8"/>
+      <c r="G183" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="H183" s="8"/>
       <c r="I183" s="8"/>
       <c r="J183" s="8"/>
       <c r="K183" s="8"/>
-      <c r="L183" s="8"/>
+      <c r="L183" s="8" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="184" spans="1:12" ht="12" thickBot="1">
       <c r="A184" s="8" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C184" s="8"/>
+        <v>81</v>
+      </c>
+      <c r="C184" s="8">
+        <v>1</v>
+      </c>
       <c r="D184" s="8"/>
       <c r="E184" s="8"/>
       <c r="F184" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G184" s="8"/>
+      <c r="G184" s="8">
+        <v>0</v>
+      </c>
       <c r="H184" s="8"/>
       <c r="I184" s="8"/>
       <c r="J184" s="8"/>
       <c r="K184" s="8"/>
-      <c r="L184" s="8" t="s">
+      <c r="L184" s="8"/>
+    </row>
+    <row r="185" spans="1:12" ht="12" thickBot="1">
+      <c r="A185" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C185" s="8"/>
+      <c r="D185" s="8"/>
+      <c r="E185" s="8"/>
+      <c r="F185" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G185" s="8"/>
+      <c r="H185" s="8"/>
+      <c r="I185" s="8"/>
+      <c r="J185" s="8"/>
+      <c r="K185" s="8"/>
+      <c r="L185" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="185" spans="1:12" ht="12" thickBot="1">
-      <c r="A185" s="10" t="s">
+    <row r="186" spans="1:12" ht="12" thickBot="1">
+      <c r="A186" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B185" s="10" t="s">
+      <c r="B186" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C185" s="10">
+      <c r="C186" s="10">
         <v>1</v>
       </c>
-      <c r="D185" s="10"/>
-      <c r="E185" s="10"/>
-      <c r="F185" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G185" s="10">
+      <c r="D186" s="10"/>
+      <c r="E186" s="10"/>
+      <c r="F186" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G186" s="10">
         <v>0</v>
       </c>
-      <c r="H185" s="10"/>
-      <c r="I185" s="10"/>
-      <c r="J185" s="10"/>
-      <c r="K185" s="10"/>
-      <c r="L185" s="10" t="s">
+      <c r="H186" s="10"/>
+      <c r="I186" s="10"/>
+      <c r="J186" s="10"/>
+      <c r="K186" s="10"/>
+      <c r="L186" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="12" thickBot="1"/>
-    <row r="187" spans="1:12" ht="12" thickBot="1">
-      <c r="A187" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B187" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C187" s="13"/>
-      <c r="D187" s="13"/>
-      <c r="E187" s="13"/>
-      <c r="F187" s="13"/>
-      <c r="G187" s="13"/>
-      <c r="H187" s="13"/>
-      <c r="I187" s="13"/>
-      <c r="J187" s="13"/>
-      <c r="K187" s="13"/>
-      <c r="L187" s="14"/>
-    </row>
+    <row r="187" spans="1:12" ht="12" thickBot="1"/>
     <row r="188" spans="1:12" ht="12" thickBot="1">
       <c r="A188" s="8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="C188" s="13"/>
       <c r="D188" s="13"/>
@@ -5673,10 +5683,12 @@
       <c r="L188" s="14"/>
     </row>
     <row r="189" spans="1:12" ht="12" thickBot="1">
-      <c r="A189" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B189" s="13"/>
+      <c r="A189" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B189" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="C189" s="13"/>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
@@ -5689,116 +5701,104 @@
       <c r="L189" s="14"/>
     </row>
     <row r="190" spans="1:12" ht="12" thickBot="1">
-      <c r="A190" s="15" t="s">
+      <c r="A190" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190" s="13"/>
+      <c r="C190" s="13"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
+      <c r="F190" s="13"/>
+      <c r="G190" s="13"/>
+      <c r="H190" s="13"/>
+      <c r="I190" s="13"/>
+      <c r="J190" s="13"/>
+      <c r="K190" s="13"/>
+      <c r="L190" s="14"/>
+    </row>
+    <row r="191" spans="1:12" ht="12" thickBot="1">
+      <c r="A191" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B190" s="15" t="s">
+      <c r="B191" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C190" s="15" t="s">
+      <c r="C191" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D190" s="15" t="s">
+      <c r="D191" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E190" s="15" t="s">
+      <c r="E191" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F190" s="15" t="s">
+      <c r="F191" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G190" s="15" t="s">
+      <c r="G191" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H190" s="17" t="s">
+      <c r="H191" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I190" s="15" t="s">
+      <c r="I191" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J190" s="12" t="s">
+      <c r="J191" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K190" s="14"/>
-      <c r="L190" s="15" t="s">
+      <c r="K191" s="14"/>
+      <c r="L191" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:12" ht="12" thickBot="1">
-      <c r="A191" s="16"/>
-      <c r="B191" s="16"/>
-      <c r="C191" s="16"/>
-      <c r="D191" s="16"/>
-      <c r="E191" s="16"/>
-      <c r="F191" s="16"/>
-      <c r="G191" s="16"/>
-      <c r="H191" s="18"/>
-      <c r="I191" s="16"/>
-      <c r="J191" s="8" t="s">
+    <row r="192" spans="1:12" ht="12" thickBot="1">
+      <c r="A192" s="16"/>
+      <c r="B192" s="16"/>
+      <c r="C192" s="16"/>
+      <c r="D192" s="16"/>
+      <c r="E192" s="16"/>
+      <c r="F192" s="16"/>
+      <c r="G192" s="16"/>
+      <c r="H192" s="18"/>
+      <c r="I192" s="16"/>
+      <c r="J192" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K191" s="8" t="s">
+      <c r="K192" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L191" s="16"/>
-    </row>
-    <row r="192" spans="1:12" ht="12" thickBot="1">
-      <c r="A192" s="10" t="s">
+      <c r="L192" s="16"/>
+    </row>
+    <row r="193" spans="1:12" ht="12" thickBot="1">
+      <c r="A193" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B192" s="10" t="s">
+      <c r="B193" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C192" s="10"/>
-      <c r="D192" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E192" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F192" s="10"/>
-      <c r="G192" s="10"/>
-      <c r="H192" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I192" s="10"/>
-      <c r="J192" s="10"/>
-      <c r="K192" s="10"/>
-      <c r="L192" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="193" spans="1:12" ht="12" thickBot="1">
-      <c r="A193" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B193" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C193" s="8">
-        <v>20</v>
-      </c>
-      <c r="D193" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E193" s="10"/>
+      <c r="C193" s="10"/>
+      <c r="D193" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E193" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F193" s="10"/>
       <c r="G193" s="10"/>
-      <c r="H193" s="10"/>
+      <c r="H193" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I193" s="10"/>
-      <c r="J193" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K193" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L193" s="8" t="s">
-        <v>103</v>
+      <c r="J193" s="10"/>
+      <c r="K193" s="10"/>
+      <c r="L193" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="194" spans="1:12" ht="12" thickBot="1">
-      <c r="A194" s="10" t="s">
-        <v>72</v>
+      <c r="A194" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B194" s="8" t="s">
         <v>102</v>
@@ -5815,7 +5815,7 @@
       <c r="H194" s="10"/>
       <c r="I194" s="10"/>
       <c r="J194" s="10" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="K194" s="10" t="s">
         <v>14</v>
@@ -5826,28 +5826,38 @@
     </row>
     <row r="195" spans="1:12" ht="12" thickBot="1">
       <c r="A195" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B195" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C195" s="10"/>
-      <c r="D195" s="10"/>
+        <v>72</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C195" s="8">
+        <v>20</v>
+      </c>
+      <c r="D195" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="E195" s="10"/>
       <c r="F195" s="10"/>
       <c r="G195" s="10"/>
       <c r="H195" s="10"/>
       <c r="I195" s="10"/>
-      <c r="J195" s="10"/>
-      <c r="K195" s="10"/>
-      <c r="L195" s="10"/>
+      <c r="J195" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K195" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L195" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="196" spans="1:12" ht="12" thickBot="1">
       <c r="A196" s="10" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B196" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C196" s="10"/>
       <c r="D196" s="10"/>
@@ -5862,7 +5872,7 @@
     </row>
     <row r="197" spans="1:12" ht="12" thickBot="1">
       <c r="A197" s="10" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B197" s="10" t="s">
         <v>85</v>
@@ -5870,9 +5880,7 @@
       <c r="C197" s="10"/>
       <c r="D197" s="10"/>
       <c r="E197" s="10"/>
-      <c r="F197" s="10" t="s">
-        <v>82</v>
-      </c>
+      <c r="F197" s="10"/>
       <c r="G197" s="10"/>
       <c r="H197" s="10"/>
       <c r="I197" s="10"/>
@@ -5882,55 +5890,57 @@
     </row>
     <row r="198" spans="1:12" ht="12" thickBot="1">
       <c r="A198" s="10" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B198" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C198" s="10">
-        <v>1</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C198" s="10"/>
       <c r="D198" s="10"/>
       <c r="E198" s="10"/>
       <c r="F198" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G198" s="10">
-        <v>0</v>
-      </c>
+      <c r="G198" s="10"/>
       <c r="H198" s="10"/>
       <c r="I198" s="10"/>
       <c r="J198" s="10"/>
       <c r="K198" s="10"/>
-      <c r="L198" s="10" t="s">
+      <c r="L198" s="10"/>
+    </row>
+    <row r="199" spans="1:12" ht="12" thickBot="1">
+      <c r="A199" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B199" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C199" s="10">
+        <v>1</v>
+      </c>
+      <c r="D199" s="10"/>
+      <c r="E199" s="10"/>
+      <c r="F199" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G199" s="10">
+        <v>0</v>
+      </c>
+      <c r="H199" s="10"/>
+      <c r="I199" s="10"/>
+      <c r="J199" s="10"/>
+      <c r="K199" s="10"/>
+      <c r="L199" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="199" spans="1:12" ht="12" thickBot="1"/>
-    <row r="200" spans="1:12" ht="12" thickBot="1">
-      <c r="A200" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B200" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C200" s="13"/>
-      <c r="D200" s="13"/>
-      <c r="E200" s="13"/>
-      <c r="F200" s="13"/>
-      <c r="G200" s="13"/>
-      <c r="H200" s="13"/>
-      <c r="I200" s="13"/>
-      <c r="J200" s="13"/>
-      <c r="K200" s="13"/>
-      <c r="L200" s="14"/>
-    </row>
+    <row r="200" spans="1:12" ht="12" thickBot="1"/>
     <row r="201" spans="1:12" ht="12" thickBot="1">
       <c r="A201" s="8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B201" s="12" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="C201" s="13"/>
       <c r="D201" s="13"/>
@@ -5944,10 +5954,12 @@
       <c r="L201" s="14"/>
     </row>
     <row r="202" spans="1:12" ht="12" thickBot="1">
-      <c r="A202" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B202" s="13"/>
+      <c r="A202" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B202" s="12" t="s">
+        <v>148</v>
+      </c>
       <c r="C202" s="13"/>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
@@ -5960,90 +5972,78 @@
       <c r="L202" s="14"/>
     </row>
     <row r="203" spans="1:12" ht="12" thickBot="1">
-      <c r="A203" s="15" t="s">
+      <c r="A203" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B203" s="13"/>
+      <c r="C203" s="13"/>
+      <c r="D203" s="13"/>
+      <c r="E203" s="13"/>
+      <c r="F203" s="13"/>
+      <c r="G203" s="13"/>
+      <c r="H203" s="13"/>
+      <c r="I203" s="13"/>
+      <c r="J203" s="13"/>
+      <c r="K203" s="13"/>
+      <c r="L203" s="14"/>
+    </row>
+    <row r="204" spans="1:12" ht="12" thickBot="1">
+      <c r="A204" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B203" s="15" t="s">
+      <c r="B204" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C203" s="15" t="s">
+      <c r="C204" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D203" s="15" t="s">
+      <c r="D204" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E203" s="15" t="s">
+      <c r="E204" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F203" s="15" t="s">
+      <c r="F204" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G203" s="15" t="s">
+      <c r="G204" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H203" s="17" t="s">
+      <c r="H204" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I203" s="15" t="s">
+      <c r="I204" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J203" s="12" t="s">
+      <c r="J204" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K203" s="14"/>
-      <c r="L203" s="15" t="s">
+      <c r="K204" s="14"/>
+      <c r="L204" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="12" thickBot="1">
-      <c r="A204" s="16"/>
-      <c r="B204" s="16"/>
-      <c r="C204" s="16"/>
-      <c r="D204" s="16"/>
-      <c r="E204" s="16"/>
-      <c r="F204" s="16"/>
-      <c r="G204" s="16"/>
-      <c r="H204" s="18"/>
-      <c r="I204" s="16"/>
-      <c r="J204" s="8" t="s">
+    <row r="205" spans="1:12" ht="12" thickBot="1">
+      <c r="A205" s="16"/>
+      <c r="B205" s="16"/>
+      <c r="C205" s="16"/>
+      <c r="D205" s="16"/>
+      <c r="E205" s="16"/>
+      <c r="F205" s="16"/>
+      <c r="G205" s="16"/>
+      <c r="H205" s="18"/>
+      <c r="I205" s="16"/>
+      <c r="J205" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K204" s="8" t="s">
+      <c r="K205" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L204" s="16"/>
-    </row>
-    <row r="205" spans="1:12" ht="12" thickBot="1">
-      <c r="A205" s="10" t="s">
+      <c r="L205" s="16"/>
+    </row>
+    <row r="206" spans="1:12" ht="12" thickBot="1">
+      <c r="A206" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="B205" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C205" s="8">
-        <v>20</v>
-      </c>
-      <c r="D205" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E205" s="10"/>
-      <c r="F205" s="10"/>
-      <c r="G205" s="10"/>
-      <c r="H205" s="10"/>
-      <c r="I205" s="10"/>
-      <c r="J205" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K205" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L205" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="206" spans="1:12" ht="12" thickBot="1">
-      <c r="A206" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="B206" s="8" t="s">
         <v>102</v>
@@ -6060,7 +6060,7 @@
       <c r="H206" s="10"/>
       <c r="I206" s="10"/>
       <c r="J206" s="10" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="K206" s="10" t="s">
         <v>14</v>
@@ -6070,56 +6070,66 @@
       </c>
     </row>
     <row r="207" spans="1:12" ht="12" thickBot="1">
-      <c r="A207" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B207" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C207" s="10">
-        <v>1</v>
-      </c>
-      <c r="D207" s="10"/>
+      <c r="A207" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C207" s="8">
+        <v>20</v>
+      </c>
+      <c r="D207" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="E207" s="10"/>
-      <c r="F207" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G207" s="10">
-        <v>0</v>
-      </c>
+      <c r="F207" s="10"/>
+      <c r="G207" s="10"/>
       <c r="H207" s="10"/>
       <c r="I207" s="10"/>
-      <c r="J207" s="10"/>
-      <c r="K207" s="10"/>
-      <c r="L207" s="10" t="s">
+      <c r="J207" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K207" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L207" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" ht="12" thickBot="1">
+      <c r="A208" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B208" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C208" s="10">
+        <v>1</v>
+      </c>
+      <c r="D208" s="10"/>
+      <c r="E208" s="10"/>
+      <c r="F208" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G208" s="10">
+        <v>0</v>
+      </c>
+      <c r="H208" s="10"/>
+      <c r="I208" s="10"/>
+      <c r="J208" s="10"/>
+      <c r="K208" s="10"/>
+      <c r="L208" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="208" spans="1:12" ht="12" thickBot="1"/>
-    <row r="209" spans="1:12" ht="12" thickBot="1">
-      <c r="A209" s="8" t="s">
+    <row r="209" spans="1:12" ht="12" thickBot="1"/>
+    <row r="210" spans="1:12" ht="12" thickBot="1">
+      <c r="A210" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B209" s="12" t="s">
+      <c r="B210" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="C209" s="13"/>
-      <c r="D209" s="13"/>
-      <c r="E209" s="13"/>
-      <c r="F209" s="13"/>
-      <c r="G209" s="13"/>
-      <c r="H209" s="13"/>
-      <c r="I209" s="13"/>
-      <c r="J209" s="13"/>
-      <c r="K209" s="13"/>
-      <c r="L209" s="14"/>
-    </row>
-    <row r="210" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A210" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B210" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="C210" s="13"/>
       <c r="D210" s="13"/>
@@ -6132,11 +6142,13 @@
       <c r="K210" s="13"/>
       <c r="L210" s="14"/>
     </row>
-    <row r="211" spans="1:12" ht="12" thickBot="1">
-      <c r="A211" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B211" s="13"/>
+    <row r="211" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A211" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B211" s="12" t="s">
+        <v>151</v>
+      </c>
       <c r="C211" s="13"/>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
@@ -6149,116 +6161,104 @@
       <c r="L211" s="14"/>
     </row>
     <row r="212" spans="1:12" ht="12" thickBot="1">
-      <c r="A212" s="15" t="s">
+      <c r="A212" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B212" s="13"/>
+      <c r="C212" s="13"/>
+      <c r="D212" s="13"/>
+      <c r="E212" s="13"/>
+      <c r="F212" s="13"/>
+      <c r="G212" s="13"/>
+      <c r="H212" s="13"/>
+      <c r="I212" s="13"/>
+      <c r="J212" s="13"/>
+      <c r="K212" s="13"/>
+      <c r="L212" s="14"/>
+    </row>
+    <row r="213" spans="1:12" ht="12" thickBot="1">
+      <c r="A213" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B212" s="15" t="s">
+      <c r="B213" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C212" s="15" t="s">
+      <c r="C213" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D212" s="15" t="s">
+      <c r="D213" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E212" s="15" t="s">
+      <c r="E213" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F212" s="15" t="s">
+      <c r="F213" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G212" s="15" t="s">
+      <c r="G213" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H212" s="17" t="s">
+      <c r="H213" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I212" s="15" t="s">
+      <c r="I213" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J212" s="12" t="s">
+      <c r="J213" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K212" s="14"/>
-      <c r="L212" s="15" t="s">
+      <c r="K213" s="14"/>
+      <c r="L213" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="12" thickBot="1">
-      <c r="A213" s="16"/>
-      <c r="B213" s="16"/>
-      <c r="C213" s="16"/>
-      <c r="D213" s="16"/>
-      <c r="E213" s="16"/>
-      <c r="F213" s="16"/>
-      <c r="G213" s="16"/>
-      <c r="H213" s="18"/>
-      <c r="I213" s="16"/>
-      <c r="J213" s="8" t="s">
+    <row r="214" spans="1:12" ht="12" thickBot="1">
+      <c r="A214" s="16"/>
+      <c r="B214" s="16"/>
+      <c r="C214" s="16"/>
+      <c r="D214" s="16"/>
+      <c r="E214" s="16"/>
+      <c r="F214" s="16"/>
+      <c r="G214" s="16"/>
+      <c r="H214" s="18"/>
+      <c r="I214" s="16"/>
+      <c r="J214" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K213" s="8" t="s">
+      <c r="K214" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L213" s="16"/>
-    </row>
-    <row r="214" spans="1:12" ht="12" thickBot="1">
-      <c r="A214" s="10" t="s">
+      <c r="L214" s="16"/>
+    </row>
+    <row r="215" spans="1:12" ht="12" thickBot="1">
+      <c r="A215" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B214" s="10" t="s">
+      <c r="B215" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C214" s="10"/>
-      <c r="D214" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E214" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F214" s="10"/>
-      <c r="G214" s="10"/>
-      <c r="H214" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I214" s="10"/>
-      <c r="J214" s="10"/>
-      <c r="K214" s="10"/>
-      <c r="L214" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="215" spans="1:12" ht="12" thickBot="1">
-      <c r="A215" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B215" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C215" s="8">
-        <v>20</v>
-      </c>
-      <c r="D215" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E215" s="10"/>
+      <c r="C215" s="10"/>
+      <c r="D215" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E215" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F215" s="10"/>
       <c r="G215" s="10"/>
-      <c r="H215" s="10"/>
+      <c r="H215" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I215" s="10"/>
-      <c r="J215" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K215" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L215" s="8" t="s">
-        <v>103</v>
+      <c r="J215" s="10"/>
+      <c r="K215" s="10"/>
+      <c r="L215" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="216" spans="1:12" ht="12" thickBot="1">
-      <c r="A216" s="10" t="s">
-        <v>60</v>
+      <c r="A216" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B216" s="8" t="s">
         <v>102</v>
@@ -6275,7 +6275,7 @@
       <c r="H216" s="10"/>
       <c r="I216" s="10"/>
       <c r="J216" s="10" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="K216" s="10" t="s">
         <v>14</v>
@@ -6286,77 +6286,87 @@
     </row>
     <row r="217" spans="1:12" ht="12" thickBot="1">
       <c r="A217" s="10" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C217" s="8"/>
-      <c r="D217" s="8"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8"/>
-      <c r="G217" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H217" s="8"/>
-      <c r="I217" s="8"/>
-      <c r="J217" s="8"/>
-      <c r="K217" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="C217" s="8">
+        <v>20</v>
+      </c>
+      <c r="D217" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E217" s="10"/>
+      <c r="F217" s="10"/>
+      <c r="G217" s="10"/>
+      <c r="H217" s="10"/>
+      <c r="I217" s="10"/>
+      <c r="J217" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K217" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="L217" s="8" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
     </row>
     <row r="218" spans="1:12" ht="12" thickBot="1">
       <c r="A218" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C218" s="8"/>
+      <c r="D218" s="8"/>
+      <c r="E218" s="8"/>
+      <c r="F218" s="8"/>
+      <c r="G218" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H218" s="8"/>
+      <c r="I218" s="8"/>
+      <c r="J218" s="8"/>
+      <c r="K218" s="8"/>
+      <c r="L218" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" ht="12" thickBot="1">
+      <c r="A219" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B218" s="10" t="s">
+      <c r="B219" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C218" s="10">
+      <c r="C219" s="10">
         <v>1</v>
       </c>
-      <c r="D218" s="10"/>
-      <c r="E218" s="10"/>
-      <c r="F218" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G218" s="10">
+      <c r="D219" s="10"/>
+      <c r="E219" s="10"/>
+      <c r="F219" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G219" s="10">
         <v>0</v>
       </c>
-      <c r="H218" s="10"/>
-      <c r="I218" s="10"/>
-      <c r="J218" s="10"/>
-      <c r="K218" s="10"/>
-      <c r="L218" s="10" t="s">
+      <c r="H219" s="10"/>
+      <c r="I219" s="10"/>
+      <c r="J219" s="10"/>
+      <c r="K219" s="10"/>
+      <c r="L219" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="219" spans="1:12" ht="12" thickBot="1"/>
-    <row r="220" spans="1:12" ht="12" thickBot="1">
-      <c r="A220" s="8" t="s">
+    <row r="220" spans="1:12" ht="12" thickBot="1"/>
+    <row r="221" spans="1:12" ht="12" thickBot="1">
+      <c r="A221" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B220" s="12" t="s">
+      <c r="B221" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="C220" s="13"/>
-      <c r="D220" s="13"/>
-      <c r="E220" s="13"/>
-      <c r="F220" s="13"/>
-      <c r="G220" s="13"/>
-      <c r="H220" s="13"/>
-      <c r="I220" s="13"/>
-      <c r="J220" s="13"/>
-      <c r="K220" s="13"/>
-      <c r="L220" s="14"/>
-    </row>
-    <row r="221" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A221" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B221" s="12" t="s">
-        <v>152</v>
       </c>
       <c r="C221" s="13"/>
       <c r="D221" s="13"/>
@@ -6369,11 +6379,13 @@
       <c r="K221" s="13"/>
       <c r="L221" s="14"/>
     </row>
-    <row r="222" spans="1:12" ht="12" thickBot="1">
-      <c r="A222" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B222" s="13"/>
+    <row r="222" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A222" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B222" s="12" t="s">
+        <v>152</v>
+      </c>
       <c r="C222" s="13"/>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
@@ -6386,116 +6398,104 @@
       <c r="L222" s="14"/>
     </row>
     <row r="223" spans="1:12" ht="12" thickBot="1">
-      <c r="A223" s="15" t="s">
+      <c r="A223" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B223" s="13"/>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="13"/>
+      <c r="F223" s="13"/>
+      <c r="G223" s="13"/>
+      <c r="H223" s="13"/>
+      <c r="I223" s="13"/>
+      <c r="J223" s="13"/>
+      <c r="K223" s="13"/>
+      <c r="L223" s="14"/>
+    </row>
+    <row r="224" spans="1:12" ht="12" thickBot="1">
+      <c r="A224" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B223" s="15" t="s">
+      <c r="B224" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C223" s="15" t="s">
+      <c r="C224" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D223" s="15" t="s">
+      <c r="D224" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E223" s="15" t="s">
+      <c r="E224" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F223" s="15" t="s">
+      <c r="F224" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G223" s="15" t="s">
+      <c r="G224" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H223" s="17" t="s">
+      <c r="H224" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I223" s="15" t="s">
+      <c r="I224" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J223" s="12" t="s">
+      <c r="J224" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K223" s="14"/>
-      <c r="L223" s="15" t="s">
+      <c r="K224" s="14"/>
+      <c r="L224" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="12" thickBot="1">
-      <c r="A224" s="16"/>
-      <c r="B224" s="16"/>
-      <c r="C224" s="16"/>
-      <c r="D224" s="16"/>
-      <c r="E224" s="16"/>
-      <c r="F224" s="16"/>
-      <c r="G224" s="16"/>
-      <c r="H224" s="18"/>
-      <c r="I224" s="16"/>
-      <c r="J224" s="8" t="s">
+    <row r="225" spans="1:12" ht="12" thickBot="1">
+      <c r="A225" s="16"/>
+      <c r="B225" s="16"/>
+      <c r="C225" s="16"/>
+      <c r="D225" s="16"/>
+      <c r="E225" s="16"/>
+      <c r="F225" s="16"/>
+      <c r="G225" s="16"/>
+      <c r="H225" s="18"/>
+      <c r="I225" s="16"/>
+      <c r="J225" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K224" s="8" t="s">
+      <c r="K225" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L224" s="16"/>
-    </row>
-    <row r="225" spans="1:12" ht="12" thickBot="1">
-      <c r="A225" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B225" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C225" s="10"/>
-      <c r="D225" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E225" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F225" s="10"/>
-      <c r="G225" s="10"/>
-      <c r="H225" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I225" s="10"/>
-      <c r="J225" s="10"/>
-      <c r="K225" s="10"/>
-      <c r="L225" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="L225" s="16"/>
     </row>
     <row r="226" spans="1:12" ht="12" thickBot="1">
       <c r="A226" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B226" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C226" s="8">
-        <v>20</v>
-      </c>
-      <c r="D226" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E226" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="B226" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C226" s="10"/>
+      <c r="D226" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E226" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F226" s="10"/>
       <c r="G226" s="10"/>
-      <c r="H226" s="10"/>
+      <c r="H226" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I226" s="10"/>
-      <c r="J226" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K226" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L226" s="8" t="s">
-        <v>103</v>
+      <c r="J226" s="10"/>
+      <c r="K226" s="10"/>
+      <c r="L226" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="227" spans="1:12" ht="12" thickBot="1">
       <c r="A227" s="10" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B227" s="8" t="s">
         <v>102</v>
@@ -6512,7 +6512,7 @@
       <c r="H227" s="10"/>
       <c r="I227" s="10"/>
       <c r="J227" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K227" s="10" t="s">
         <v>14</v>
@@ -6523,55 +6523,65 @@
     </row>
     <row r="228" spans="1:12" ht="12" thickBot="1">
       <c r="A228" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B228" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C228" s="10">
-        <v>1</v>
-      </c>
-      <c r="D228" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C228" s="8">
+        <v>20</v>
+      </c>
+      <c r="D228" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="E228" s="10"/>
-      <c r="F228" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G228" s="10">
-        <v>0</v>
-      </c>
+      <c r="F228" s="10"/>
+      <c r="G228" s="10"/>
       <c r="H228" s="10"/>
       <c r="I228" s="10"/>
-      <c r="J228" s="10"/>
-      <c r="K228" s="10"/>
-      <c r="L228" s="10" t="s">
+      <c r="J228" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K228" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L228" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" ht="12" thickBot="1">
+      <c r="A229" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B229" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C229" s="10">
+        <v>1</v>
+      </c>
+      <c r="D229" s="10"/>
+      <c r="E229" s="10"/>
+      <c r="F229" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G229" s="10">
+        <v>0</v>
+      </c>
+      <c r="H229" s="10"/>
+      <c r="I229" s="10"/>
+      <c r="J229" s="10"/>
+      <c r="K229" s="10"/>
+      <c r="L229" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="229" spans="1:12" ht="12" thickBot="1"/>
-    <row r="230" spans="1:12" ht="12" thickBot="1">
-      <c r="A230" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B230" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C230" s="13"/>
-      <c r="D230" s="13"/>
-      <c r="E230" s="13"/>
-      <c r="F230" s="13"/>
-      <c r="G230" s="13"/>
-      <c r="H230" s="13"/>
-      <c r="I230" s="13"/>
-      <c r="J230" s="13"/>
-      <c r="K230" s="13"/>
-      <c r="L230" s="14"/>
-    </row>
+    <row r="230" spans="1:12" ht="12" thickBot="1"/>
     <row r="231" spans="1:12" ht="12" thickBot="1">
       <c r="A231" s="8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B231" s="12" t="s">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="C231" s="13"/>
       <c r="D231" s="13"/>
@@ -6585,10 +6595,12 @@
       <c r="L231" s="14"/>
     </row>
     <row r="232" spans="1:12" ht="12" thickBot="1">
-      <c r="A232" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B232" s="13"/>
+      <c r="A232" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B232" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="C232" s="13"/>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
@@ -6601,117 +6613,115 @@
       <c r="L232" s="14"/>
     </row>
     <row r="233" spans="1:12" ht="12" thickBot="1">
-      <c r="A233" s="15" t="s">
+      <c r="A233" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B233" s="13"/>
+      <c r="C233" s="13"/>
+      <c r="D233" s="13"/>
+      <c r="E233" s="13"/>
+      <c r="F233" s="13"/>
+      <c r="G233" s="13"/>
+      <c r="H233" s="13"/>
+      <c r="I233" s="13"/>
+      <c r="J233" s="13"/>
+      <c r="K233" s="13"/>
+      <c r="L233" s="14"/>
+    </row>
+    <row r="234" spans="1:12" ht="12" thickBot="1">
+      <c r="A234" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B233" s="15" t="s">
+      <c r="B234" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C233" s="15" t="s">
+      <c r="C234" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D233" s="15" t="s">
+      <c r="D234" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E233" s="15" t="s">
+      <c r="E234" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F233" s="15" t="s">
+      <c r="F234" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G233" s="15" t="s">
+      <c r="G234" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H233" s="17" t="s">
+      <c r="H234" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="I233" s="15" t="s">
+      <c r="I234" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="J233" s="12" t="s">
+      <c r="J234" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K233" s="14"/>
-      <c r="L233" s="15" t="s">
+      <c r="K234" s="14"/>
+      <c r="L234" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:12" ht="12" thickBot="1">
-      <c r="A234" s="16"/>
-      <c r="B234" s="16"/>
-      <c r="C234" s="16"/>
-      <c r="D234" s="16"/>
-      <c r="E234" s="16"/>
-      <c r="F234" s="16"/>
-      <c r="G234" s="16"/>
-      <c r="H234" s="18"/>
-      <c r="I234" s="16"/>
-      <c r="J234" s="8" t="s">
+    <row r="235" spans="1:12" ht="12" thickBot="1">
+      <c r="A235" s="16"/>
+      <c r="B235" s="16"/>
+      <c r="C235" s="16"/>
+      <c r="D235" s="16"/>
+      <c r="E235" s="16"/>
+      <c r="F235" s="16"/>
+      <c r="G235" s="16"/>
+      <c r="H235" s="18"/>
+      <c r="I235" s="16"/>
+      <c r="J235" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="K234" s="8" t="s">
+      <c r="K235" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="L234" s="16"/>
-    </row>
-    <row r="235" spans="1:12" ht="12" thickBot="1">
-      <c r="A235" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B235" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C235" s="10"/>
-      <c r="D235" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E235" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F235" s="10"/>
-      <c r="G235" s="10"/>
-      <c r="H235" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I235" s="10"/>
-      <c r="J235" s="10"/>
-      <c r="K235" s="10"/>
-      <c r="L235" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="L235" s="16"/>
     </row>
     <row r="236" spans="1:12" ht="12" thickBot="1">
       <c r="A236" s="10" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B236" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C236" s="10">
-        <v>15</v>
-      </c>
-      <c r="D236" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="C236" s="10"/>
+      <c r="D236" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="E236" s="10" t="s">
         <v>82</v>
       </c>
       <c r="F236" s="10"/>
       <c r="G236" s="10"/>
-      <c r="H236" s="10"/>
+      <c r="H236" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I236" s="10"/>
       <c r="J236" s="10"/>
       <c r="K236" s="10"/>
-      <c r="L236" s="10"/>
+      <c r="L236" s="10" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="237" spans="1:12" ht="12" thickBot="1">
       <c r="A237" s="10" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B237" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C237" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="C237" s="10">
+        <v>15</v>
+      </c>
       <c r="D237" s="10"/>
-      <c r="E237" s="10"/>
+      <c r="E237" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="F237" s="10"/>
       <c r="G237" s="10"/>
       <c r="H237" s="10"/>
@@ -6721,8 +6731,8 @@
       <c r="L237" s="10"/>
     </row>
     <row r="238" spans="1:12" ht="12" thickBot="1">
-      <c r="A238" s="8" t="s">
-        <v>153</v>
+      <c r="A238" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="B238" s="10" t="s">
         <v>85</v>
@@ -6732,43 +6742,39 @@
       <c r="E238" s="10"/>
       <c r="F238" s="10"/>
       <c r="G238" s="10"/>
-      <c r="H238" s="10" t="s">
-        <v>82</v>
-      </c>
+      <c r="H238" s="10"/>
       <c r="I238" s="10"/>
-      <c r="J238" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K238" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L238" s="8"/>
-    </row>
-    <row r="239" spans="1:12" ht="34.5" thickBot="1">
+      <c r="J238" s="10"/>
+      <c r="K238" s="10"/>
+      <c r="L238" s="10"/>
+    </row>
+    <row r="239" spans="1:12" ht="12" thickBot="1">
       <c r="A239" s="8" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="B239" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C239" s="10">
-        <v>15</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C239" s="10"/>
       <c r="D239" s="10"/>
       <c r="E239" s="10"/>
       <c r="F239" s="10"/>
       <c r="G239" s="10"/>
-      <c r="H239" s="10"/>
+      <c r="H239" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="I239" s="10"/>
-      <c r="J239" s="10"/>
-      <c r="K239" s="10"/>
-      <c r="L239" s="8" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="240" spans="1:12" ht="12" thickBot="1">
+      <c r="J239" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K239" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L239" s="8"/>
+    </row>
+    <row r="240" spans="1:12" ht="34.5" thickBot="1">
       <c r="A240" s="8" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B240" s="10" t="s">
         <v>79</v>
@@ -6784,61 +6790,55 @@
       <c r="I240" s="10"/>
       <c r="J240" s="10"/>
       <c r="K240" s="10"/>
-      <c r="L240" s="8"/>
+      <c r="L240" s="8" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="241" spans="1:12" ht="12" thickBot="1">
       <c r="A241" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B241" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C241" s="8"/>
-      <c r="D241" s="8"/>
-      <c r="E241" s="8"/>
-      <c r="F241" s="8"/>
-      <c r="G241" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H241" s="8"/>
-      <c r="I241" s="8"/>
-      <c r="J241" s="8"/>
-      <c r="K241" s="8"/>
-      <c r="L241" s="8" t="s">
-        <v>150</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B241" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C241" s="10">
+        <v>15</v>
+      </c>
+      <c r="D241" s="10"/>
+      <c r="E241" s="10"/>
+      <c r="F241" s="10"/>
+      <c r="G241" s="10"/>
+      <c r="H241" s="10"/>
+      <c r="I241" s="10"/>
+      <c r="J241" s="10"/>
+      <c r="K241" s="10"/>
+      <c r="L241" s="8"/>
     </row>
     <row r="242" spans="1:12" ht="12" thickBot="1">
       <c r="A242" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C242" s="8"/>
+      <c r="D242" s="8"/>
+      <c r="E242" s="8"/>
+      <c r="F242" s="8"/>
+      <c r="G242" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H242" s="8"/>
+      <c r="I242" s="8"/>
+      <c r="J242" s="8"/>
+      <c r="K242" s="8"/>
+      <c r="L242" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" ht="12" thickBot="1">
+      <c r="A243" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="B242" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C242" s="10">
-        <v>1</v>
-      </c>
-      <c r="D242" s="10"/>
-      <c r="E242" s="10"/>
-      <c r="F242" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G242" s="10"/>
-      <c r="H242" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I242" s="10"/>
-      <c r="J242" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="K242" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L242" s="8"/>
-    </row>
-    <row r="243" spans="1:12" ht="12" thickBot="1">
-      <c r="A243" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="B243" s="10" t="s">
         <v>81</v>
@@ -6851,240 +6851,61 @@
       <c r="F243" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G243" s="10">
+      <c r="G243" s="10"/>
+      <c r="H243" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I243" s="10"/>
+      <c r="J243" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K243" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L243" s="8"/>
+    </row>
+    <row r="244" spans="1:12" ht="12" thickBot="1">
+      <c r="A244" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B244" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C244" s="10">
+        <v>1</v>
+      </c>
+      <c r="D244" s="10"/>
+      <c r="E244" s="10"/>
+      <c r="F244" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G244" s="10">
         <v>0</v>
       </c>
-      <c r="H243" s="10"/>
-      <c r="I243" s="10"/>
-      <c r="J243" s="10"/>
-      <c r="K243" s="10"/>
-      <c r="L243" s="10" t="s">
+      <c r="H244" s="10"/>
+      <c r="I244" s="10"/>
+      <c r="J244" s="10"/>
+      <c r="K244" s="10"/>
+      <c r="L244" s="10" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="252">
-    <mergeCell ref="B230:L230"/>
-    <mergeCell ref="B231:L231"/>
-    <mergeCell ref="A232:L232"/>
-    <mergeCell ref="A233:A234"/>
-    <mergeCell ref="B233:B234"/>
-    <mergeCell ref="C233:C234"/>
-    <mergeCell ref="D233:D234"/>
-    <mergeCell ref="E233:E234"/>
-    <mergeCell ref="F233:F234"/>
-    <mergeCell ref="G233:G234"/>
-    <mergeCell ref="I233:I234"/>
-    <mergeCell ref="J233:K233"/>
-    <mergeCell ref="L233:L234"/>
-    <mergeCell ref="H233:H234"/>
-    <mergeCell ref="B220:L220"/>
-    <mergeCell ref="B221:L221"/>
-    <mergeCell ref="A222:L222"/>
-    <mergeCell ref="A223:A224"/>
-    <mergeCell ref="B223:B224"/>
-    <mergeCell ref="C223:C224"/>
-    <mergeCell ref="D223:D224"/>
-    <mergeCell ref="E223:E224"/>
-    <mergeCell ref="F223:F224"/>
-    <mergeCell ref="G223:G224"/>
-    <mergeCell ref="I223:I224"/>
-    <mergeCell ref="J223:K223"/>
-    <mergeCell ref="L223:L224"/>
-    <mergeCell ref="H223:H224"/>
-    <mergeCell ref="B210:L210"/>
-    <mergeCell ref="B209:L209"/>
-    <mergeCell ref="A211:L211"/>
-    <mergeCell ref="A212:A213"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:C213"/>
-    <mergeCell ref="D212:D213"/>
-    <mergeCell ref="E212:E213"/>
-    <mergeCell ref="F212:F213"/>
-    <mergeCell ref="G212:G213"/>
-    <mergeCell ref="I212:I213"/>
-    <mergeCell ref="J212:K212"/>
-    <mergeCell ref="L212:L213"/>
-    <mergeCell ref="H212:H213"/>
-    <mergeCell ref="B200:L200"/>
-    <mergeCell ref="B201:L201"/>
-    <mergeCell ref="A202:L202"/>
-    <mergeCell ref="A203:A204"/>
-    <mergeCell ref="B203:B204"/>
-    <mergeCell ref="C203:C204"/>
-    <mergeCell ref="D203:D204"/>
-    <mergeCell ref="E203:E204"/>
-    <mergeCell ref="F203:F204"/>
-    <mergeCell ref="G203:G204"/>
-    <mergeCell ref="I203:I204"/>
-    <mergeCell ref="J203:K203"/>
-    <mergeCell ref="L203:L204"/>
-    <mergeCell ref="H203:H204"/>
-    <mergeCell ref="B187:L187"/>
-    <mergeCell ref="B188:L188"/>
-    <mergeCell ref="A189:L189"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="C190:C191"/>
-    <mergeCell ref="D190:D191"/>
-    <mergeCell ref="E190:E191"/>
-    <mergeCell ref="F190:F191"/>
-    <mergeCell ref="G190:G191"/>
-    <mergeCell ref="I190:I191"/>
-    <mergeCell ref="J190:K190"/>
-    <mergeCell ref="L190:L191"/>
-    <mergeCell ref="H190:H191"/>
-    <mergeCell ref="B173:L173"/>
-    <mergeCell ref="B174:L174"/>
-    <mergeCell ref="A175:L175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="B176:B177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="D176:D177"/>
-    <mergeCell ref="E176:E177"/>
-    <mergeCell ref="F176:F177"/>
-    <mergeCell ref="G176:G177"/>
-    <mergeCell ref="I176:I177"/>
-    <mergeCell ref="J176:K176"/>
-    <mergeCell ref="L176:L177"/>
-    <mergeCell ref="H176:H177"/>
-    <mergeCell ref="B158:L158"/>
-    <mergeCell ref="B159:L159"/>
-    <mergeCell ref="A160:L160"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="C161:C162"/>
-    <mergeCell ref="D161:D162"/>
-    <mergeCell ref="E161:E162"/>
-    <mergeCell ref="F161:F162"/>
-    <mergeCell ref="G161:G162"/>
-    <mergeCell ref="I161:I162"/>
-    <mergeCell ref="J161:K161"/>
-    <mergeCell ref="L161:L162"/>
-    <mergeCell ref="H161:H162"/>
-    <mergeCell ref="B110:L110"/>
-    <mergeCell ref="B111:L111"/>
-    <mergeCell ref="A112:L112"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="E113:E114"/>
-    <mergeCell ref="F113:F114"/>
-    <mergeCell ref="G113:G114"/>
-    <mergeCell ref="I113:I114"/>
-    <mergeCell ref="J113:K113"/>
-    <mergeCell ref="L113:L114"/>
-    <mergeCell ref="H113:H114"/>
-    <mergeCell ref="B101:L101"/>
-    <mergeCell ref="B102:L102"/>
-    <mergeCell ref="A103:L103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="G104:G105"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="L104:L105"/>
-    <mergeCell ref="H104:H105"/>
-    <mergeCell ref="B89:L89"/>
-    <mergeCell ref="B90:L90"/>
-    <mergeCell ref="A91:L91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="G92:G93"/>
-    <mergeCell ref="I92:I93"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="L92:L93"/>
-    <mergeCell ref="H92:H93"/>
-    <mergeCell ref="B128:L128"/>
-    <mergeCell ref="B129:L129"/>
-    <mergeCell ref="A130:L130"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="F131:F132"/>
-    <mergeCell ref="G131:G132"/>
-    <mergeCell ref="I131:I132"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="L131:L132"/>
-    <mergeCell ref="H131:H132"/>
-    <mergeCell ref="B76:L76"/>
-    <mergeCell ref="B77:L77"/>
-    <mergeCell ref="A78:L78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="L79:L80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A40:L40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="B68:L68"/>
-    <mergeCell ref="B69:L69"/>
-    <mergeCell ref="A70:L70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="I71:I72"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="I51:I52"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="L51:L52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="B145:L145"/>
+    <mergeCell ref="B146:L146"/>
+    <mergeCell ref="A147:L147"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="B148:B149"/>
+    <mergeCell ref="C148:C149"/>
+    <mergeCell ref="D148:D149"/>
+    <mergeCell ref="E148:E149"/>
+    <mergeCell ref="F148:F149"/>
+    <mergeCell ref="G148:G149"/>
+    <mergeCell ref="H148:H149"/>
+    <mergeCell ref="I148:I149"/>
+    <mergeCell ref="J148:K148"/>
+    <mergeCell ref="L148:L149"/>
     <mergeCell ref="B30:L30"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="A32:L32"/>
@@ -7102,20 +6923,227 @@
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="H33:H34"/>
-    <mergeCell ref="B144:L144"/>
-    <mergeCell ref="B145:L145"/>
-    <mergeCell ref="A146:L146"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="H147:H148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="L147:L148"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="I51:I52"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:L52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="B68:L68"/>
+    <mergeCell ref="B69:L69"/>
+    <mergeCell ref="A70:L70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="I71:I72"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B39:L39"/>
+    <mergeCell ref="A40:L40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="B76:L76"/>
+    <mergeCell ref="B77:L77"/>
+    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="L79:L80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="B129:L129"/>
+    <mergeCell ref="B130:L130"/>
+    <mergeCell ref="A131:L131"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="I132:I133"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="L132:L133"/>
+    <mergeCell ref="H132:H133"/>
+    <mergeCell ref="B89:L89"/>
+    <mergeCell ref="B90:L90"/>
+    <mergeCell ref="A91:L91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="G92:G93"/>
+    <mergeCell ref="I92:I93"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="L92:L93"/>
+    <mergeCell ref="H92:H93"/>
+    <mergeCell ref="B101:L101"/>
+    <mergeCell ref="B102:L102"/>
+    <mergeCell ref="A103:L103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="G104:G105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="L104:L105"/>
+    <mergeCell ref="H104:H105"/>
+    <mergeCell ref="B110:L110"/>
+    <mergeCell ref="B111:L111"/>
+    <mergeCell ref="A112:L112"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="G113:G114"/>
+    <mergeCell ref="I113:I114"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="L113:L114"/>
+    <mergeCell ref="H113:H114"/>
+    <mergeCell ref="B159:L159"/>
+    <mergeCell ref="B160:L160"/>
+    <mergeCell ref="A161:L161"/>
+    <mergeCell ref="A162:A163"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="C162:C163"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="G162:G163"/>
+    <mergeCell ref="I162:I163"/>
+    <mergeCell ref="J162:K162"/>
+    <mergeCell ref="L162:L163"/>
+    <mergeCell ref="H162:H163"/>
+    <mergeCell ref="B174:L174"/>
+    <mergeCell ref="B175:L175"/>
+    <mergeCell ref="A176:L176"/>
+    <mergeCell ref="A177:A178"/>
+    <mergeCell ref="B177:B178"/>
+    <mergeCell ref="C177:C178"/>
+    <mergeCell ref="D177:D178"/>
+    <mergeCell ref="E177:E178"/>
+    <mergeCell ref="F177:F178"/>
+    <mergeCell ref="G177:G178"/>
+    <mergeCell ref="I177:I178"/>
+    <mergeCell ref="J177:K177"/>
+    <mergeCell ref="L177:L178"/>
+    <mergeCell ref="H177:H178"/>
+    <mergeCell ref="B188:L188"/>
+    <mergeCell ref="B189:L189"/>
+    <mergeCell ref="A190:L190"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="B191:B192"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="D191:D192"/>
+    <mergeCell ref="E191:E192"/>
+    <mergeCell ref="F191:F192"/>
+    <mergeCell ref="G191:G192"/>
+    <mergeCell ref="I191:I192"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="L191:L192"/>
+    <mergeCell ref="H191:H192"/>
+    <mergeCell ref="B201:L201"/>
+    <mergeCell ref="B202:L202"/>
+    <mergeCell ref="A203:L203"/>
+    <mergeCell ref="A204:A205"/>
+    <mergeCell ref="B204:B205"/>
+    <mergeCell ref="C204:C205"/>
+    <mergeCell ref="D204:D205"/>
+    <mergeCell ref="E204:E205"/>
+    <mergeCell ref="F204:F205"/>
+    <mergeCell ref="G204:G205"/>
+    <mergeCell ref="I204:I205"/>
+    <mergeCell ref="J204:K204"/>
+    <mergeCell ref="L204:L205"/>
+    <mergeCell ref="H204:H205"/>
+    <mergeCell ref="B211:L211"/>
+    <mergeCell ref="B210:L210"/>
+    <mergeCell ref="A212:L212"/>
+    <mergeCell ref="A213:A214"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="C213:C214"/>
+    <mergeCell ref="D213:D214"/>
+    <mergeCell ref="E213:E214"/>
+    <mergeCell ref="F213:F214"/>
+    <mergeCell ref="G213:G214"/>
+    <mergeCell ref="I213:I214"/>
+    <mergeCell ref="J213:K213"/>
+    <mergeCell ref="L213:L214"/>
+    <mergeCell ref="H213:H214"/>
+    <mergeCell ref="B221:L221"/>
+    <mergeCell ref="B222:L222"/>
+    <mergeCell ref="A223:L223"/>
+    <mergeCell ref="A224:A225"/>
+    <mergeCell ref="B224:B225"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="D224:D225"/>
+    <mergeCell ref="E224:E225"/>
+    <mergeCell ref="F224:F225"/>
+    <mergeCell ref="G224:G225"/>
+    <mergeCell ref="I224:I225"/>
+    <mergeCell ref="J224:K224"/>
+    <mergeCell ref="L224:L225"/>
+    <mergeCell ref="H224:H225"/>
+    <mergeCell ref="B231:L231"/>
+    <mergeCell ref="B232:L232"/>
+    <mergeCell ref="A233:L233"/>
+    <mergeCell ref="A234:A235"/>
+    <mergeCell ref="B234:B235"/>
+    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="D234:D235"/>
+    <mergeCell ref="E234:E235"/>
+    <mergeCell ref="F234:F235"/>
+    <mergeCell ref="G234:G235"/>
+    <mergeCell ref="I234:I235"/>
+    <mergeCell ref="J234:K234"/>
+    <mergeCell ref="L234:L235"/>
+    <mergeCell ref="H234:H235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -7126,8 +7154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="F286" sqref="F286"/>
+    <sheetView topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="D260" sqref="D260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12884,6 +12912,216 @@
     </row>
   </sheetData>
   <mergeCells count="220">
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="B80:G80"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="B90:G90"/>
+    <mergeCell ref="B91:G91"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="G93:G94"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B106:G106"/>
+    <mergeCell ref="A107:G107"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="B121:G121"/>
+    <mergeCell ref="B122:G122"/>
+    <mergeCell ref="A123:G123"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="B139:G139"/>
+    <mergeCell ref="B140:G140"/>
+    <mergeCell ref="A141:G141"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="E142:E143"/>
+    <mergeCell ref="F142:F143"/>
+    <mergeCell ref="G142:G143"/>
+    <mergeCell ref="B147:G147"/>
+    <mergeCell ref="B148:G148"/>
+    <mergeCell ref="A149:G149"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="D150:D151"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="F150:F151"/>
+    <mergeCell ref="G150:G151"/>
+    <mergeCell ref="B186:G186"/>
+    <mergeCell ref="B187:G187"/>
+    <mergeCell ref="A188:G188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="B189:B190"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="E189:E190"/>
+    <mergeCell ref="F189:F190"/>
+    <mergeCell ref="G189:G190"/>
+    <mergeCell ref="B233:G233"/>
+    <mergeCell ref="B234:G234"/>
+    <mergeCell ref="A235:G235"/>
+    <mergeCell ref="A236:A237"/>
+    <mergeCell ref="B236:B237"/>
+    <mergeCell ref="C236:C237"/>
+    <mergeCell ref="D236:D237"/>
+    <mergeCell ref="E236:E237"/>
+    <mergeCell ref="F236:F237"/>
+    <mergeCell ref="G236:G237"/>
+    <mergeCell ref="B244:G244"/>
+    <mergeCell ref="B245:G245"/>
+    <mergeCell ref="A246:G246"/>
+    <mergeCell ref="A247:A248"/>
+    <mergeCell ref="B247:B248"/>
+    <mergeCell ref="C247:C248"/>
+    <mergeCell ref="D247:D248"/>
+    <mergeCell ref="E247:E248"/>
+    <mergeCell ref="F247:F248"/>
+    <mergeCell ref="G247:G248"/>
+    <mergeCell ref="B255:G255"/>
+    <mergeCell ref="B256:G256"/>
+    <mergeCell ref="A257:G257"/>
+    <mergeCell ref="A258:A259"/>
+    <mergeCell ref="B258:B259"/>
+    <mergeCell ref="C258:C259"/>
+    <mergeCell ref="D258:D259"/>
+    <mergeCell ref="E258:E259"/>
+    <mergeCell ref="F258:F259"/>
+    <mergeCell ref="G258:G259"/>
+    <mergeCell ref="B268:G268"/>
+    <mergeCell ref="B269:G269"/>
+    <mergeCell ref="A270:G270"/>
+    <mergeCell ref="A271:A272"/>
+    <mergeCell ref="B271:B272"/>
+    <mergeCell ref="C271:C272"/>
+    <mergeCell ref="D271:D272"/>
+    <mergeCell ref="E271:E272"/>
+    <mergeCell ref="F271:F272"/>
+    <mergeCell ref="G271:G272"/>
+    <mergeCell ref="B287:G287"/>
+    <mergeCell ref="B288:G288"/>
+    <mergeCell ref="A289:G289"/>
+    <mergeCell ref="A290:A291"/>
+    <mergeCell ref="B290:B291"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="D290:D291"/>
+    <mergeCell ref="E290:E291"/>
+    <mergeCell ref="F290:F291"/>
+    <mergeCell ref="G290:G291"/>
+    <mergeCell ref="B305:G305"/>
+    <mergeCell ref="B306:G306"/>
+    <mergeCell ref="A307:G307"/>
+    <mergeCell ref="A308:A309"/>
+    <mergeCell ref="B308:B309"/>
+    <mergeCell ref="C308:C309"/>
+    <mergeCell ref="D308:D309"/>
+    <mergeCell ref="E308:E309"/>
+    <mergeCell ref="F308:F309"/>
+    <mergeCell ref="G308:G309"/>
+    <mergeCell ref="B333:G333"/>
+    <mergeCell ref="B334:G334"/>
+    <mergeCell ref="A335:G335"/>
+    <mergeCell ref="A336:A337"/>
+    <mergeCell ref="B336:B337"/>
+    <mergeCell ref="C336:C337"/>
+    <mergeCell ref="D336:D337"/>
+    <mergeCell ref="E336:E337"/>
+    <mergeCell ref="F336:F337"/>
+    <mergeCell ref="G336:G337"/>
     <mergeCell ref="B343:G343"/>
     <mergeCell ref="B344:G344"/>
     <mergeCell ref="A345:G345"/>
@@ -12894,216 +13132,6 @@
     <mergeCell ref="E346:E347"/>
     <mergeCell ref="F346:F347"/>
     <mergeCell ref="G346:G347"/>
-    <mergeCell ref="B333:G333"/>
-    <mergeCell ref="B334:G334"/>
-    <mergeCell ref="A335:G335"/>
-    <mergeCell ref="A336:A337"/>
-    <mergeCell ref="B336:B337"/>
-    <mergeCell ref="C336:C337"/>
-    <mergeCell ref="D336:D337"/>
-    <mergeCell ref="E336:E337"/>
-    <mergeCell ref="F336:F337"/>
-    <mergeCell ref="G336:G337"/>
-    <mergeCell ref="B305:G305"/>
-    <mergeCell ref="B306:G306"/>
-    <mergeCell ref="A307:G307"/>
-    <mergeCell ref="A308:A309"/>
-    <mergeCell ref="B308:B309"/>
-    <mergeCell ref="C308:C309"/>
-    <mergeCell ref="D308:D309"/>
-    <mergeCell ref="E308:E309"/>
-    <mergeCell ref="F308:F309"/>
-    <mergeCell ref="G308:G309"/>
-    <mergeCell ref="B287:G287"/>
-    <mergeCell ref="B288:G288"/>
-    <mergeCell ref="A289:G289"/>
-    <mergeCell ref="A290:A291"/>
-    <mergeCell ref="B290:B291"/>
-    <mergeCell ref="C290:C291"/>
-    <mergeCell ref="D290:D291"/>
-    <mergeCell ref="E290:E291"/>
-    <mergeCell ref="F290:F291"/>
-    <mergeCell ref="G290:G291"/>
-    <mergeCell ref="B268:G268"/>
-    <mergeCell ref="B269:G269"/>
-    <mergeCell ref="A270:G270"/>
-    <mergeCell ref="A271:A272"/>
-    <mergeCell ref="B271:B272"/>
-    <mergeCell ref="C271:C272"/>
-    <mergeCell ref="D271:D272"/>
-    <mergeCell ref="E271:E272"/>
-    <mergeCell ref="F271:F272"/>
-    <mergeCell ref="G271:G272"/>
-    <mergeCell ref="B255:G255"/>
-    <mergeCell ref="B256:G256"/>
-    <mergeCell ref="A257:G257"/>
-    <mergeCell ref="A258:A259"/>
-    <mergeCell ref="B258:B259"/>
-    <mergeCell ref="C258:C259"/>
-    <mergeCell ref="D258:D259"/>
-    <mergeCell ref="E258:E259"/>
-    <mergeCell ref="F258:F259"/>
-    <mergeCell ref="G258:G259"/>
-    <mergeCell ref="B244:G244"/>
-    <mergeCell ref="B245:G245"/>
-    <mergeCell ref="A246:G246"/>
-    <mergeCell ref="A247:A248"/>
-    <mergeCell ref="B247:B248"/>
-    <mergeCell ref="C247:C248"/>
-    <mergeCell ref="D247:D248"/>
-    <mergeCell ref="E247:E248"/>
-    <mergeCell ref="F247:F248"/>
-    <mergeCell ref="G247:G248"/>
-    <mergeCell ref="B233:G233"/>
-    <mergeCell ref="B234:G234"/>
-    <mergeCell ref="A235:G235"/>
-    <mergeCell ref="A236:A237"/>
-    <mergeCell ref="B236:B237"/>
-    <mergeCell ref="C236:C237"/>
-    <mergeCell ref="D236:D237"/>
-    <mergeCell ref="E236:E237"/>
-    <mergeCell ref="F236:F237"/>
-    <mergeCell ref="G236:G237"/>
-    <mergeCell ref="B186:G186"/>
-    <mergeCell ref="B187:G187"/>
-    <mergeCell ref="A188:G188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="B189:B190"/>
-    <mergeCell ref="C189:C190"/>
-    <mergeCell ref="D189:D190"/>
-    <mergeCell ref="E189:E190"/>
-    <mergeCell ref="F189:F190"/>
-    <mergeCell ref="G189:G190"/>
-    <mergeCell ref="B147:G147"/>
-    <mergeCell ref="B148:G148"/>
-    <mergeCell ref="A149:G149"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="D150:D151"/>
-    <mergeCell ref="E150:E151"/>
-    <mergeCell ref="F150:F151"/>
-    <mergeCell ref="G150:G151"/>
-    <mergeCell ref="B139:G139"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="A141:G141"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="E142:E143"/>
-    <mergeCell ref="F142:F143"/>
-    <mergeCell ref="G142:G143"/>
-    <mergeCell ref="B121:G121"/>
-    <mergeCell ref="B122:G122"/>
-    <mergeCell ref="A123:G123"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="G124:G125"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B106:G106"/>
-    <mergeCell ref="A107:G107"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="B90:G90"/>
-    <mergeCell ref="B91:G91"/>
-    <mergeCell ref="A92:G92"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="G93:G94"/>
-    <mergeCell ref="B79:G79"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>